<commit_message>
Update modelling configuration (add custom constraint for ramp up/down as a sample)
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/gen.xlsx
+++ b/spine_rts-gmlc/datasets/gen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="gen" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9697" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10017" uniqueCount="443">
   <si>
     <t>GEN UID</t>
   </si>
@@ -1344,13 +1344,28 @@
   <si>
     <t>313_HEAD_STORAGE</t>
   </si>
+  <si>
+    <t>para_name_7</t>
+  </si>
+  <si>
+    <t>para_name_8</t>
+  </si>
+  <si>
+    <t>value [MW/h]</t>
+  </si>
+  <si>
+    <t>ramp_up</t>
+  </si>
+  <si>
+    <t>ramp_down</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1835,13 +1850,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2166,10 +2182,10 @@
   <dimension ref="A1:BD159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO4" sqref="AO4"/>
+      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29243,10 +29259,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O159"/>
+  <dimension ref="A1:S159"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I159"/>
+    <sheetView topLeftCell="H139" workbookViewId="0">
+      <selection activeCell="R159" sqref="R2:S159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29266,9 +29282,10 @@
     <col min="13" max="13" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -29314,8 +29331,20 @@
       <c r="O1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>440</v>
+      </c>
+      <c r="R1" t="s">
+        <v>439</v>
+      </c>
+      <c r="S1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -29368,8 +29397,22 @@
         <f>VLOOKUP(A2,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC2+VLOOKUP(A2,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>VLOOKUP(A2,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R2" t="s">
+        <v>442</v>
+      </c>
+      <c r="S2" s="6">
+        <f>VLOOKUP(A2,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -29422,8 +29465,22 @@
         <f>VLOOKUP(A3,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC3+VLOOKUP(A3,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P3" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>VLOOKUP(A3,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R3" t="s">
+        <v>442</v>
+      </c>
+      <c r="S3" s="6">
+        <f>VLOOKUP(A3,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -29476,8 +29533,22 @@
         <f>VLOOKUP(A4,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC4+VLOOKUP(A4,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>11172.014352</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P4" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>VLOOKUP(A4,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+      <c r="R4" t="s">
+        <v>442</v>
+      </c>
+      <c r="S4" s="6">
+        <f>VLOOKUP(A4,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -29530,8 +29601,22 @@
         <f>VLOOKUP(A5,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC5+VLOOKUP(A5,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>11172.014352</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P5" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>VLOOKUP(A5,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+      <c r="R5" t="s">
+        <v>442</v>
+      </c>
+      <c r="S5" s="6">
+        <f>VLOOKUP(A5,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -29584,8 +29669,22 @@
         <f>VLOOKUP(A6,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC6+VLOOKUP(A6,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P6" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>VLOOKUP(A6,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R6" t="s">
+        <v>442</v>
+      </c>
+      <c r="S6" s="6">
+        <f>VLOOKUP(A6,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -29638,8 +29737,22 @@
         <f>VLOOKUP(A7,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC7+VLOOKUP(A7,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P7" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q7" s="2">
+        <f>VLOOKUP(A7,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R7" t="s">
+        <v>442</v>
+      </c>
+      <c r="S7" s="6">
+        <f>VLOOKUP(A7,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -29692,8 +29805,22 @@
         <f>VLOOKUP(A8,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC8+VLOOKUP(A8,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>11172.014352</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P8" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q8" s="2">
+        <f>VLOOKUP(A8,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+      <c r="R8" t="s">
+        <v>442</v>
+      </c>
+      <c r="S8" s="6">
+        <f>VLOOKUP(A8,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -29746,8 +29873,22 @@
         <f>VLOOKUP(A9,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC9+VLOOKUP(A9,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>11172.014352</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P9" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q9" s="2">
+        <f>VLOOKUP(A9,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+      <c r="R9" t="s">
+        <v>442</v>
+      </c>
+      <c r="S9" s="6">
+        <f>VLOOKUP(A9,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -29800,8 +29941,22 @@
         <f>VLOOKUP(A10,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC10+VLOOKUP(A10,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P10" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q10" s="2">
+        <f>VLOOKUP(A10,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R10" t="s">
+        <v>442</v>
+      </c>
+      <c r="S10" s="6">
+        <f>VLOOKUP(A10,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>78</v>
       </c>
@@ -29854,8 +30009,22 @@
         <f>VLOOKUP(A11,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC11+VLOOKUP(A11,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P11" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q11" s="2">
+        <f>VLOOKUP(A11,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R11" t="s">
+        <v>442</v>
+      </c>
+      <c r="S11" s="6">
+        <f>VLOOKUP(A11,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -29908,8 +30077,22 @@
         <f>VLOOKUP(A12,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC12+VLOOKUP(A12,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P12" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q12" s="2">
+        <f>VLOOKUP(A12,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R12" t="s">
+        <v>442</v>
+      </c>
+      <c r="S12" s="6">
+        <f>VLOOKUP(A12,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -29962,8 +30145,22 @@
         <f>VLOOKUP(A13,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC13+VLOOKUP(A13,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P13" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q13" s="2">
+        <f>VLOOKUP(A13,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R13" t="s">
+        <v>442</v>
+      </c>
+      <c r="S13" s="6">
+        <f>VLOOKUP(A13,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -30016,8 +30213,22 @@
         <f>VLOOKUP(A14,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC14+VLOOKUP(A14,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P14" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q14" s="2">
+        <f>VLOOKUP(A14,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R14" t="s">
+        <v>442</v>
+      </c>
+      <c r="S14" s="6">
+        <f>VLOOKUP(A14,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -30070,8 +30281,22 @@
         <f>VLOOKUP(A15,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC15+VLOOKUP(A15,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>703.75919999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P15" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q15" s="2">
+        <f>VLOOKUP(A15,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+      <c r="R15" t="s">
+        <v>442</v>
+      </c>
+      <c r="S15" s="6">
+        <f>VLOOKUP(A15,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -30124,8 +30349,22 @@
         <f>VLOOKUP(A16,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC16+VLOOKUP(A16,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>703.75919999999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P16" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q16" s="2">
+        <f>VLOOKUP(A16,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+      <c r="R16" t="s">
+        <v>442</v>
+      </c>
+      <c r="S16" s="6">
+        <f>VLOOKUP(A16,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -30178,8 +30417,22 @@
         <f>VLOOKUP(A17,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC17+VLOOKUP(A17,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>22784.795619</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P17" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q17" s="2">
+        <f>VLOOKUP(A17,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R17" t="s">
+        <v>442</v>
+      </c>
+      <c r="S17" s="6">
+        <f>VLOOKUP(A17,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -30232,8 +30485,22 @@
         <f>VLOOKUP(A18,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC18+VLOOKUP(A18,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>22784.795619</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P18" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q18" s="2">
+        <f>VLOOKUP(A18,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R18" t="s">
+        <v>442</v>
+      </c>
+      <c r="S18" s="6">
+        <f>VLOOKUP(A18,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -30286,8 +30553,22 @@
         <f>VLOOKUP(A19,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC19+VLOOKUP(A19,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P19" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q19" s="2">
+        <f>VLOOKUP(A19,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R19" t="s">
+        <v>442</v>
+      </c>
+      <c r="S19" s="6">
+        <f>VLOOKUP(A19,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -30340,8 +30621,22 @@
         <f>VLOOKUP(A20,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC20+VLOOKUP(A20,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>22784.795619</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P20" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q20" s="2">
+        <f>VLOOKUP(A20,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R20" t="s">
+        <v>442</v>
+      </c>
+      <c r="S20" s="6">
+        <f>VLOOKUP(A20,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -30394,8 +30689,22 @@
         <f>VLOOKUP(A21,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC21+VLOOKUP(A21,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>36749.813558999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P21" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q21" s="2">
+        <f>VLOOKUP(A21,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>240</v>
+      </c>
+      <c r="R21" t="s">
+        <v>442</v>
+      </c>
+      <c r="S21" s="6">
+        <f>VLOOKUP(A21,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>96</v>
       </c>
@@ -30448,8 +30757,22 @@
         <f>VLOOKUP(A22,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC22+VLOOKUP(A22,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P22" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q22" s="2">
+        <f>VLOOKUP(A22,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R22" t="s">
+        <v>442</v>
+      </c>
+      <c r="S22" s="6">
+        <f>VLOOKUP(A22,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -30502,8 +30825,22 @@
         <f>VLOOKUP(A23,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC23+VLOOKUP(A23,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P23" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q23" s="2">
+        <f>VLOOKUP(A23,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R23" t="s">
+        <v>442</v>
+      </c>
+      <c r="S23" s="6">
+        <f>VLOOKUP(A23,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -30556,8 +30893,22 @@
         <f>VLOOKUP(A24,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC24+VLOOKUP(A24,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P24" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q24" s="2">
+        <f>VLOOKUP(A24,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R24" t="s">
+        <v>442</v>
+      </c>
+      <c r="S24" s="6">
+        <f>VLOOKUP(A24,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -30610,8 +30961,22 @@
         <f>VLOOKUP(A25,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC25+VLOOKUP(A25,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P25" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q25" s="2">
+        <f>VLOOKUP(A25,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R25" t="s">
+        <v>442</v>
+      </c>
+      <c r="S25" s="6">
+        <f>VLOOKUP(A25,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -30664,8 +31029,22 @@
         <f>VLOOKUP(A26,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC26+VLOOKUP(A26,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P26" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q26" s="2">
+        <f>VLOOKUP(A26,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R26" t="s">
+        <v>442</v>
+      </c>
+      <c r="S26" s="6">
+        <f>VLOOKUP(A26,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -30718,8 +31097,22 @@
         <f>VLOOKUP(A27,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC27+VLOOKUP(A27,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>11172.014352</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P27" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q27" s="2">
+        <f>VLOOKUP(A27,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+      <c r="R27" t="s">
+        <v>442</v>
+      </c>
+      <c r="S27" s="6">
+        <f>VLOOKUP(A27,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -30772,8 +31165,22 @@
         <f>VLOOKUP(A28,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC28+VLOOKUP(A28,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P28" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q28" s="2">
+        <f>VLOOKUP(A28,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R28" t="s">
+        <v>442</v>
+      </c>
+      <c r="S28" s="6">
+        <f>VLOOKUP(A28,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -30826,8 +31233,22 @@
         <f>VLOOKUP(A29,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC29+VLOOKUP(A29,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P29" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q29" s="2">
+        <f>VLOOKUP(A29,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R29" t="s">
+        <v>442</v>
+      </c>
+      <c r="S29" s="6">
+        <f>VLOOKUP(A29,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -30880,8 +31301,22 @@
         <f>VLOOKUP(A30,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC30+VLOOKUP(A30,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>11172.014352</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P30" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q30" s="2">
+        <f>VLOOKUP(A30,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+      <c r="R30" t="s">
+        <v>442</v>
+      </c>
+      <c r="S30" s="6">
+        <f>VLOOKUP(A30,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -30934,8 +31369,22 @@
         <f>VLOOKUP(A31,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC31+VLOOKUP(A31,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>11172.014352</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P31" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q31" s="2">
+        <f>VLOOKUP(A31,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+      <c r="R31" t="s">
+        <v>442</v>
+      </c>
+      <c r="S31" s="6">
+        <f>VLOOKUP(A31,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>106</v>
       </c>
@@ -30988,8 +31437,22 @@
         <f>VLOOKUP(A32,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC32+VLOOKUP(A32,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P32" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q32" s="2">
+        <f>VLOOKUP(A32,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R32" t="s">
+        <v>442</v>
+      </c>
+      <c r="S32" s="6">
+        <f>VLOOKUP(A32,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -31042,8 +31505,22 @@
         <f>VLOOKUP(A33,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC33+VLOOKUP(A33,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P33" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q33" s="2">
+        <f>VLOOKUP(A33,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R33" t="s">
+        <v>442</v>
+      </c>
+      <c r="S33" s="6">
+        <f>VLOOKUP(A33,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -31096,8 +31573,22 @@
         <f>VLOOKUP(A34,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC34+VLOOKUP(A34,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P34" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q34" s="2">
+        <f>VLOOKUP(A34,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R34" t="s">
+        <v>442</v>
+      </c>
+      <c r="S34" s="6">
+        <f>VLOOKUP(A34,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -31150,8 +31641,22 @@
         <f>VLOOKUP(A35,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC35+VLOOKUP(A35,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P35" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q35" s="2">
+        <f>VLOOKUP(A35,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R35" t="s">
+        <v>442</v>
+      </c>
+      <c r="S35" s="6">
+        <f>VLOOKUP(A35,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>110</v>
       </c>
@@ -31204,8 +31709,22 @@
         <f>VLOOKUP(A36,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC36+VLOOKUP(A36,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P36" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q36" s="2">
+        <f>VLOOKUP(A36,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R36" t="s">
+        <v>442</v>
+      </c>
+      <c r="S36" s="6">
+        <f>VLOOKUP(A36,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>111</v>
       </c>
@@ -31258,8 +31777,22 @@
         <f>VLOOKUP(A37,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC37+VLOOKUP(A37,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P37" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q37" s="2">
+        <f>VLOOKUP(A37,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R37" t="s">
+        <v>442</v>
+      </c>
+      <c r="S37" s="6">
+        <f>VLOOKUP(A37,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -31312,8 +31845,22 @@
         <f>VLOOKUP(A38,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC38+VLOOKUP(A38,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P38" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q38" s="2">
+        <f>VLOOKUP(A38,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R38" t="s">
+        <v>442</v>
+      </c>
+      <c r="S38" s="6">
+        <f>VLOOKUP(A38,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>113</v>
       </c>
@@ -31366,8 +31913,22 @@
         <f>VLOOKUP(A39,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC39+VLOOKUP(A39,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>22784.795619</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P39" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q39" s="2">
+        <f>VLOOKUP(A39,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R39" t="s">
+        <v>442</v>
+      </c>
+      <c r="S39" s="6">
+        <f>VLOOKUP(A39,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>114</v>
       </c>
@@ -31420,8 +31981,22 @@
         <f>VLOOKUP(A40,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC40+VLOOKUP(A40,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P40" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q40" s="2">
+        <f>VLOOKUP(A40,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R40" t="s">
+        <v>442</v>
+      </c>
+      <c r="S40" s="6">
+        <f>VLOOKUP(A40,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>115</v>
       </c>
@@ -31474,8 +32049,22 @@
         <f>VLOOKUP(A41,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC41+VLOOKUP(A41,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P41" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q41" s="2">
+        <f>VLOOKUP(A41,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R41" t="s">
+        <v>442</v>
+      </c>
+      <c r="S41" s="6">
+        <f>VLOOKUP(A41,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>116</v>
       </c>
@@ -31528,8 +32117,22 @@
         <f>VLOOKUP(A42,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC42+VLOOKUP(A42,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>22784.795619</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P42" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q42" s="2">
+        <f>VLOOKUP(A42,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R42" t="s">
+        <v>442</v>
+      </c>
+      <c r="S42" s="6">
+        <f>VLOOKUP(A42,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>117</v>
       </c>
@@ -31582,8 +32185,22 @@
         <f>VLOOKUP(A43,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC43+VLOOKUP(A43,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>22784.795619</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P43" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q43" s="2">
+        <f>VLOOKUP(A43,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R43" t="s">
+        <v>442</v>
+      </c>
+      <c r="S43" s="6">
+        <f>VLOOKUP(A43,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>118</v>
       </c>
@@ -31636,8 +32253,22 @@
         <f>VLOOKUP(A44,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC44+VLOOKUP(A44,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>36749.813558999995</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P44" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q44" s="2">
+        <f>VLOOKUP(A44,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>240</v>
+      </c>
+      <c r="R44" t="s">
+        <v>442</v>
+      </c>
+      <c r="S44" s="6">
+        <f>VLOOKUP(A44,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>119</v>
       </c>
@@ -31690,8 +32321,22 @@
         <f>VLOOKUP(A45,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC45+VLOOKUP(A45,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P45" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q45" s="2">
+        <f>VLOOKUP(A45,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R45" t="s">
+        <v>442</v>
+      </c>
+      <c r="S45" s="6">
+        <f>VLOOKUP(A45,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>120</v>
       </c>
@@ -31744,8 +32389,22 @@
         <f>VLOOKUP(A46,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC46+VLOOKUP(A46,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P46" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q46" s="2">
+        <f>VLOOKUP(A46,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R46" t="s">
+        <v>442</v>
+      </c>
+      <c r="S46" s="6">
+        <f>VLOOKUP(A46,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>121</v>
       </c>
@@ -31798,8 +32457,22 @@
         <f>VLOOKUP(A47,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC47+VLOOKUP(A47,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P47" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q47" s="2">
+        <f>VLOOKUP(A47,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R47" t="s">
+        <v>442</v>
+      </c>
+      <c r="S47" s="6">
+        <f>VLOOKUP(A47,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>122</v>
       </c>
@@ -31852,8 +32525,22 @@
         <f>VLOOKUP(A48,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC48+VLOOKUP(A48,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P48" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q48" s="2">
+        <f>VLOOKUP(A48,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R48" t="s">
+        <v>442</v>
+      </c>
+      <c r="S48" s="6">
+        <f>VLOOKUP(A48,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>123</v>
       </c>
@@ -31906,8 +32593,22 @@
         <f>VLOOKUP(A49,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC49+VLOOKUP(A49,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P49" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q49" s="2">
+        <f>VLOOKUP(A49,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R49" t="s">
+        <v>442</v>
+      </c>
+      <c r="S49" s="6">
+        <f>VLOOKUP(A49,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -31960,8 +32661,22 @@
         <f>VLOOKUP(A50,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC50+VLOOKUP(A50,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P50" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q50" s="2">
+        <f>VLOOKUP(A50,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R50" t="s">
+        <v>442</v>
+      </c>
+      <c r="S50" s="6">
+        <f>VLOOKUP(A50,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>125</v>
       </c>
@@ -32014,8 +32729,22 @@
         <f>VLOOKUP(A51,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC51+VLOOKUP(A51,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P51" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q51" s="2">
+        <f>VLOOKUP(A51,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R51" t="s">
+        <v>442</v>
+      </c>
+      <c r="S51" s="6">
+        <f>VLOOKUP(A51,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>126</v>
       </c>
@@ -32068,8 +32797,22 @@
         <f>VLOOKUP(A52,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC52+VLOOKUP(A52,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P52" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q52" s="2">
+        <f>VLOOKUP(A52,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R52" t="s">
+        <v>442</v>
+      </c>
+      <c r="S52" s="6">
+        <f>VLOOKUP(A52,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>127</v>
       </c>
@@ -32122,8 +32865,22 @@
         <f>VLOOKUP(A53,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC53+VLOOKUP(A53,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>51.747</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P53" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q53" s="2">
+        <f>VLOOKUP(A53,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R53" t="s">
+        <v>442</v>
+      </c>
+      <c r="S53" s="6">
+        <f>VLOOKUP(A53,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>128</v>
       </c>
@@ -32176,8 +32933,22 @@
         <f>VLOOKUP(A54,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC54+VLOOKUP(A54,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P54" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q54" s="2">
+        <f>VLOOKUP(A54,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R54" t="s">
+        <v>442</v>
+      </c>
+      <c r="S54" s="6">
+        <f>VLOOKUP(A54,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>129</v>
       </c>
@@ -32230,8 +33001,22 @@
         <f>VLOOKUP(A55,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC55+VLOOKUP(A55,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P55" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q55" s="2">
+        <f>VLOOKUP(A55,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R55" t="s">
+        <v>442</v>
+      </c>
+      <c r="S55" s="6">
+        <f>VLOOKUP(A55,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>130</v>
       </c>
@@ -32284,8 +33069,22 @@
         <f>VLOOKUP(A56,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC56+VLOOKUP(A56,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P56" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q56" s="2">
+        <f>VLOOKUP(A56,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R56" t="s">
+        <v>442</v>
+      </c>
+      <c r="S56" s="6">
+        <f>VLOOKUP(A56,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>131</v>
       </c>
@@ -32338,8 +33137,22 @@
         <f>VLOOKUP(A57,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC57+VLOOKUP(A57,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P57" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q57" s="2">
+        <f>VLOOKUP(A57,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R57" t="s">
+        <v>442</v>
+      </c>
+      <c r="S57" s="6">
+        <f>VLOOKUP(A57,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>132</v>
       </c>
@@ -32392,8 +33205,22 @@
         <f>VLOOKUP(A58,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC58+VLOOKUP(A58,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P58" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q58" s="2">
+        <f>VLOOKUP(A58,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R58" t="s">
+        <v>442</v>
+      </c>
+      <c r="S58" s="6">
+        <f>VLOOKUP(A58,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>133</v>
       </c>
@@ -32446,8 +33273,22 @@
         <f>VLOOKUP(A59,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC59+VLOOKUP(A59,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>703.75919999999996</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P59" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q59" s="2">
+        <f>VLOOKUP(A59,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+      <c r="R59" t="s">
+        <v>442</v>
+      </c>
+      <c r="S59" s="6">
+        <f>VLOOKUP(A59,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>134</v>
       </c>
@@ -32500,8 +33341,22 @@
         <f>VLOOKUP(A60,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC60+VLOOKUP(A60,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>703.75919999999996</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P60" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q60" s="2">
+        <f>VLOOKUP(A60,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+      <c r="R60" t="s">
+        <v>442</v>
+      </c>
+      <c r="S60" s="6">
+        <f>VLOOKUP(A60,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>135</v>
       </c>
@@ -32554,8 +33409,22 @@
         <f>VLOOKUP(A61,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC61+VLOOKUP(A61,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>703.75919999999996</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P61" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q61" s="2">
+        <f>VLOOKUP(A61,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+      <c r="R61" t="s">
+        <v>442</v>
+      </c>
+      <c r="S61" s="6">
+        <f>VLOOKUP(A61,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>136</v>
       </c>
@@ -32608,8 +33477,22 @@
         <f>VLOOKUP(A62,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC62+VLOOKUP(A62,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>703.75919999999996</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P62" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q62" s="2">
+        <f>VLOOKUP(A62,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+      <c r="R62" t="s">
+        <v>442</v>
+      </c>
+      <c r="S62" s="6">
+        <f>VLOOKUP(A62,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>137</v>
       </c>
@@ -32662,8 +33545,22 @@
         <f>VLOOKUP(A63,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC63+VLOOKUP(A63,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>703.75919999999996</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P63" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q63" s="2">
+        <f>VLOOKUP(A63,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+      <c r="R63" t="s">
+        <v>442</v>
+      </c>
+      <c r="S63" s="6">
+        <f>VLOOKUP(A63,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>138</v>
       </c>
@@ -32716,8 +33613,22 @@
         <f>VLOOKUP(A64,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC64+VLOOKUP(A64,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P64" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q64" s="2">
+        <f>VLOOKUP(A64,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R64" t="s">
+        <v>442</v>
+      </c>
+      <c r="S64" s="6">
+        <f>VLOOKUP(A64,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>139</v>
       </c>
@@ -32770,8 +33681,22 @@
         <f>VLOOKUP(A65,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC65+VLOOKUP(A65,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P65" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q65" s="2">
+        <f>VLOOKUP(A65,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R65" t="s">
+        <v>442</v>
+      </c>
+      <c r="S65" s="6">
+        <f>VLOOKUP(A65,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>140</v>
       </c>
@@ -32824,8 +33749,22 @@
         <f>VLOOKUP(A66,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC66+VLOOKUP(A66,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P66" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q66" s="2">
+        <f>VLOOKUP(A66,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R66" t="s">
+        <v>442</v>
+      </c>
+      <c r="S66" s="6">
+        <f>VLOOKUP(A66,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -32878,8 +33817,22 @@
         <f>VLOOKUP(A67,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC67+VLOOKUP(A67,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>22784.795619</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P67" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q67" s="2">
+        <f>VLOOKUP(A67,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+      <c r="R67" t="s">
+        <v>442</v>
+      </c>
+      <c r="S67" s="6">
+        <f>VLOOKUP(A67,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>142</v>
       </c>
@@ -32932,8 +33885,22 @@
         <f>VLOOKUP(A68,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC68+VLOOKUP(A68,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P68" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q68" s="2">
+        <f>VLOOKUP(A68,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R68" t="s">
+        <v>442</v>
+      </c>
+      <c r="S68" s="6">
+        <f>VLOOKUP(A68,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>143</v>
       </c>
@@ -32986,8 +33953,22 @@
         <f>VLOOKUP(A69,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC69+VLOOKUP(A69,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P69" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q69" s="2">
+        <f>VLOOKUP(A69,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R69" t="s">
+        <v>442</v>
+      </c>
+      <c r="S69" s="6">
+        <f>VLOOKUP(A69,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>144</v>
       </c>
@@ -33040,8 +34021,22 @@
         <f>VLOOKUP(A70,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC70+VLOOKUP(A70,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P70" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q70" s="2">
+        <f>VLOOKUP(A70,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R70" t="s">
+        <v>442</v>
+      </c>
+      <c r="S70" s="6">
+        <f>VLOOKUP(A70,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>145</v>
       </c>
@@ -33094,8 +34089,22 @@
         <f>VLOOKUP(A71,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC71+VLOOKUP(A71,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>5665.2344280000007</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P71" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q71" s="2">
+        <f>VLOOKUP(A71,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+      <c r="R71" t="s">
+        <v>442</v>
+      </c>
+      <c r="S71" s="6">
+        <f>VLOOKUP(A71,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>146</v>
       </c>
@@ -33148,8 +34157,22 @@
         <f>VLOOKUP(A72,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC72+VLOOKUP(A72,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P72" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q72" s="2">
+        <f>VLOOKUP(A72,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R72" t="s">
+        <v>442</v>
+      </c>
+      <c r="S72" s="6">
+        <f>VLOOKUP(A72,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>147</v>
       </c>
@@ -33202,8 +34225,22 @@
         <f>VLOOKUP(A73,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC73+VLOOKUP(A73,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>28046.681022000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P73" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q73" s="2">
+        <f>VLOOKUP(A73,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+      <c r="R73" t="s">
+        <v>442</v>
+      </c>
+      <c r="S73" s="6">
+        <f>VLOOKUP(A73,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>248.39999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>148</v>
       </c>
@@ -33256,8 +34293,22 @@
         <f>VLOOKUP(A74,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC74+VLOOKUP(A74,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P74" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q74" s="2">
+        <f>VLOOKUP(A74,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>0</v>
+      </c>
+      <c r="R74" t="s">
+        <v>442</v>
+      </c>
+      <c r="S74" s="6">
+        <f>VLOOKUP(A74,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>151</v>
       </c>
@@ -33310,8 +34361,22 @@
         <f>VLOOKUP(A75,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC75+VLOOKUP(A75,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>63999.8223</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P75" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q75" s="2">
+        <f>VLOOKUP(A75,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1200</v>
+      </c>
+      <c r="R75" t="s">
+        <v>442</v>
+      </c>
+      <c r="S75" s="6">
+        <f>VLOOKUP(A75,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>155</v>
       </c>
@@ -33364,8 +34429,22 @@
         <f>VLOOKUP(A76,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC76+VLOOKUP(A76,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P76" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q76" s="2">
+        <f>VLOOKUP(A76,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R76" t="s">
+        <v>442</v>
+      </c>
+      <c r="S76" s="6">
+        <f>VLOOKUP(A76,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>159</v>
       </c>
@@ -33418,8 +34497,22 @@
         <f>VLOOKUP(A77,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC77+VLOOKUP(A77,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P77" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q77" s="2">
+        <f>VLOOKUP(A77,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R77" t="s">
+        <v>442</v>
+      </c>
+      <c r="S77" s="6">
+        <f>VLOOKUP(A77,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>160</v>
       </c>
@@ -33472,8 +34565,22 @@
         <f>VLOOKUP(A78,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC78+VLOOKUP(A78,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P78" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q78" s="2">
+        <f>VLOOKUP(A78,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R78" t="s">
+        <v>442</v>
+      </c>
+      <c r="S78" s="6">
+        <f>VLOOKUP(A78,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>161</v>
       </c>
@@ -33526,8 +34633,22 @@
         <f>VLOOKUP(A79,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC79+VLOOKUP(A79,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P79" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q79" s="2">
+        <f>VLOOKUP(A79,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R79" t="s">
+        <v>442</v>
+      </c>
+      <c r="S79" s="6">
+        <f>VLOOKUP(A79,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>162</v>
       </c>
@@ -33580,8 +34701,22 @@
         <f>VLOOKUP(A80,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC80+VLOOKUP(A80,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P80" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q80" s="2">
+        <f>VLOOKUP(A80,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R80" t="s">
+        <v>442</v>
+      </c>
+      <c r="S80" s="6">
+        <f>VLOOKUP(A80,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -33634,8 +34769,22 @@
         <f>VLOOKUP(A81,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC81+VLOOKUP(A81,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P81" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q81" s="2">
+        <f>VLOOKUP(A81,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R81" t="s">
+        <v>442</v>
+      </c>
+      <c r="S81" s="6">
+        <f>VLOOKUP(A81,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>164</v>
       </c>
@@ -33688,8 +34837,22 @@
         <f>VLOOKUP(A82,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC82+VLOOKUP(A82,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P82" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q82" s="2">
+        <f>VLOOKUP(A82,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R82" t="s">
+        <v>442</v>
+      </c>
+      <c r="S82" s="6">
+        <f>VLOOKUP(A82,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -33742,8 +34905,22 @@
         <f>VLOOKUP(A83,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC83+VLOOKUP(A83,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P83" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q83" s="2">
+        <f>VLOOKUP(A83,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>0</v>
+      </c>
+      <c r="R83" t="s">
+        <v>442</v>
+      </c>
+      <c r="S83" s="6">
+        <f>VLOOKUP(A83,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>166</v>
       </c>
@@ -33796,8 +34973,22 @@
         <f>VLOOKUP(A84,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC84+VLOOKUP(A84,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P84" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q84" s="2">
+        <f>VLOOKUP(A84,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R84" t="s">
+        <v>442</v>
+      </c>
+      <c r="S84" s="6">
+        <f>VLOOKUP(A84,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>167</v>
       </c>
@@ -33850,8 +35041,22 @@
         <f>VLOOKUP(A85,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC85+VLOOKUP(A85,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P85" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q85" s="2">
+        <f>VLOOKUP(A85,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R85" t="s">
+        <v>442</v>
+      </c>
+      <c r="S85" s="6">
+        <f>VLOOKUP(A85,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -33904,8 +35109,22 @@
         <f>VLOOKUP(A86,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC86+VLOOKUP(A86,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P86" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q86" s="2">
+        <f>VLOOKUP(A86,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R86" t="s">
+        <v>442</v>
+      </c>
+      <c r="S86" s="6">
+        <f>VLOOKUP(A86,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -33958,8 +35177,22 @@
         <f>VLOOKUP(A87,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC87+VLOOKUP(A87,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P87" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q87" s="2">
+        <f>VLOOKUP(A87,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R87" t="s">
+        <v>442</v>
+      </c>
+      <c r="S87" s="6">
+        <f>VLOOKUP(A87,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>170</v>
       </c>
@@ -34012,8 +35245,22 @@
         <f>VLOOKUP(A88,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC88+VLOOKUP(A88,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P88" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q88" s="2">
+        <f>VLOOKUP(A88,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R88" t="s">
+        <v>442</v>
+      </c>
+      <c r="S88" s="6">
+        <f>VLOOKUP(A88,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>171</v>
       </c>
@@ -34066,8 +35313,22 @@
         <f>VLOOKUP(A89,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC89+VLOOKUP(A89,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P89" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q89" s="2">
+        <f>VLOOKUP(A89,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R89" t="s">
+        <v>442</v>
+      </c>
+      <c r="S89" s="6">
+        <f>VLOOKUP(A89,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -34120,8 +35381,22 @@
         <f>VLOOKUP(A90,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC90+VLOOKUP(A90,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P90" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q90" s="2">
+        <f>VLOOKUP(A90,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R90" t="s">
+        <v>442</v>
+      </c>
+      <c r="S90" s="6">
+        <f>VLOOKUP(A90,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>173</v>
       </c>
@@ -34174,8 +35449,22 @@
         <f>VLOOKUP(A91,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC91+VLOOKUP(A91,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P91" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q91" s="2">
+        <f>VLOOKUP(A91,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R91" t="s">
+        <v>442</v>
+      </c>
+      <c r="S91" s="6">
+        <f>VLOOKUP(A91,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>174</v>
       </c>
@@ -34228,8 +35517,22 @@
         <f>VLOOKUP(A92,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC92+VLOOKUP(A92,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P92" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q92" s="2">
+        <f>VLOOKUP(A92,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R92" t="s">
+        <v>442</v>
+      </c>
+      <c r="S92" s="6">
+        <f>VLOOKUP(A92,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>175</v>
       </c>
@@ -34282,8 +35585,22 @@
         <f>VLOOKUP(A93,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC93+VLOOKUP(A93,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P93" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q93" s="2">
+        <f>VLOOKUP(A93,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>0</v>
+      </c>
+      <c r="R93" t="s">
+        <v>442</v>
+      </c>
+      <c r="S93" s="6">
+        <f>VLOOKUP(A93,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>176</v>
       </c>
@@ -34336,8 +35653,22 @@
         <f>VLOOKUP(A94,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC94+VLOOKUP(A94,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P94" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q94" s="2">
+        <f>VLOOKUP(A94,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R94" t="s">
+        <v>442</v>
+      </c>
+      <c r="S94" s="6">
+        <f>VLOOKUP(A94,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -34390,8 +35721,22 @@
         <f>VLOOKUP(A95,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC95+VLOOKUP(A95,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P95" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q95" s="2">
+        <f>VLOOKUP(A95,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R95" t="s">
+        <v>442</v>
+      </c>
+      <c r="S95" s="6">
+        <f>VLOOKUP(A95,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>178</v>
       </c>
@@ -34444,8 +35789,22 @@
         <f>VLOOKUP(A96,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC96+VLOOKUP(A96,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P96" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q96" s="2">
+        <f>VLOOKUP(A96,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R96" t="s">
+        <v>442</v>
+      </c>
+      <c r="S96" s="6">
+        <f>VLOOKUP(A96,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>179</v>
       </c>
@@ -34498,8 +35857,22 @@
         <f>VLOOKUP(A97,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC97+VLOOKUP(A97,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P97" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q97" s="2">
+        <f>VLOOKUP(A97,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R97" t="s">
+        <v>442</v>
+      </c>
+      <c r="S97" s="6">
+        <f>VLOOKUP(A97,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>180</v>
       </c>
@@ -34552,8 +35925,22 @@
         <f>VLOOKUP(A98,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC98+VLOOKUP(A98,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P98" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q98" s="2">
+        <f>VLOOKUP(A98,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+      <c r="R98" t="s">
+        <v>442</v>
+      </c>
+      <c r="S98" s="6">
+        <f>VLOOKUP(A98,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>184</v>
       </c>
@@ -34606,8 +35993,22 @@
         <f>VLOOKUP(A99,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC99+VLOOKUP(A99,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P99" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q99" s="2">
+        <f>VLOOKUP(A99,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+      <c r="R99" t="s">
+        <v>442</v>
+      </c>
+      <c r="S99" s="6">
+        <f>VLOOKUP(A99,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -34660,8 +36061,22 @@
         <f>VLOOKUP(A100,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC100+VLOOKUP(A100,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P100" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q100" s="2">
+        <f>VLOOKUP(A100,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+      <c r="R100" t="s">
+        <v>442</v>
+      </c>
+      <c r="S100" s="6">
+        <f>VLOOKUP(A100,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>186</v>
       </c>
@@ -34714,8 +36129,22 @@
         <f>VLOOKUP(A101,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC101+VLOOKUP(A101,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P101" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q101" s="2">
+        <f>VLOOKUP(A101,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5706</v>
+      </c>
+      <c r="R101" t="s">
+        <v>442</v>
+      </c>
+      <c r="S101" s="6">
+        <f>VLOOKUP(A101,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5706</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>187</v>
       </c>
@@ -34768,8 +36197,22 @@
         <f>VLOOKUP(A102,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC102+VLOOKUP(A102,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P102" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q102" s="2">
+        <f>VLOOKUP(A102,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5562</v>
+      </c>
+      <c r="R102" t="s">
+        <v>442</v>
+      </c>
+      <c r="S102" s="6">
+        <f>VLOOKUP(A102,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5562</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>188</v>
       </c>
@@ -34822,8 +36265,22 @@
         <f>VLOOKUP(A103,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC103+VLOOKUP(A103,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P103" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q103" s="2">
+        <f>VLOOKUP(A103,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+      <c r="R103" t="s">
+        <v>442</v>
+      </c>
+      <c r="S103" s="6">
+        <f>VLOOKUP(A103,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>189</v>
       </c>
@@ -34876,8 +36333,22 @@
         <f>VLOOKUP(A104,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC104+VLOOKUP(A104,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P104" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q104" s="2">
+        <f>VLOOKUP(A104,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5598</v>
+      </c>
+      <c r="R104" t="s">
+        <v>442</v>
+      </c>
+      <c r="S104" s="6">
+        <f>VLOOKUP(A104,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5598</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>190</v>
       </c>
@@ -34930,8 +36401,22 @@
         <f>VLOOKUP(A105,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC105+VLOOKUP(A105,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P105" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q105" s="2">
+        <f>VLOOKUP(A105,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3102</v>
+      </c>
+      <c r="R105" t="s">
+        <v>442</v>
+      </c>
+      <c r="S105" s="6">
+        <f>VLOOKUP(A105,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>191</v>
       </c>
@@ -34984,8 +36469,22 @@
         <f>VLOOKUP(A106,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC106+VLOOKUP(A106,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P106" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q106" s="2">
+        <f>VLOOKUP(A106,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>2982</v>
+      </c>
+      <c r="R106" t="s">
+        <v>442</v>
+      </c>
+      <c r="S106" s="6">
+        <f>VLOOKUP(A106,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>2982</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>192</v>
       </c>
@@ -35038,8 +36537,22 @@
         <f>VLOOKUP(A107,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC107+VLOOKUP(A107,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P107" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q107" s="2">
+        <f>VLOOKUP(A107,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5646</v>
+      </c>
+      <c r="R107" t="s">
+        <v>442</v>
+      </c>
+      <c r="S107" s="6">
+        <f>VLOOKUP(A107,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5646</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>193</v>
       </c>
@@ -35092,8 +36605,22 @@
         <f>VLOOKUP(A108,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC108+VLOOKUP(A108,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P108" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q108" s="2">
+        <f>VLOOKUP(A108,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+      <c r="R108" t="s">
+        <v>442</v>
+      </c>
+      <c r="S108" s="6">
+        <f>VLOOKUP(A108,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>194</v>
       </c>
@@ -35146,8 +36673,22 @@
         <f>VLOOKUP(A109,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC109+VLOOKUP(A109,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P109" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q109" s="2">
+        <f>VLOOKUP(A109,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+      <c r="R109" t="s">
+        <v>442</v>
+      </c>
+      <c r="S109" s="6">
+        <f>VLOOKUP(A109,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>195</v>
       </c>
@@ -35200,8 +36741,22 @@
         <f>VLOOKUP(A110,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC110+VLOOKUP(A110,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P110" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q110" s="2">
+        <f>VLOOKUP(A110,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3060</v>
+      </c>
+      <c r="R110" t="s">
+        <v>442</v>
+      </c>
+      <c r="S110" s="6">
+        <f>VLOOKUP(A110,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>196</v>
       </c>
@@ -35254,8 +36809,22 @@
         <f>VLOOKUP(A111,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC111+VLOOKUP(A111,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P111" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q111" s="2">
+        <f>VLOOKUP(A111,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5616</v>
+      </c>
+      <c r="R111" t="s">
+        <v>442</v>
+      </c>
+      <c r="S111" s="6">
+        <f>VLOOKUP(A111,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>5616</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>197</v>
       </c>
@@ -35308,8 +36877,22 @@
         <f>VLOOKUP(A112,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC112+VLOOKUP(A112,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P112" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q112" s="2">
+        <f>VLOOKUP(A112,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>11292</v>
+      </c>
+      <c r="R112" t="s">
+        <v>442</v>
+      </c>
+      <c r="S112" s="6">
+        <f>VLOOKUP(A112,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>11292</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>198</v>
       </c>
@@ -35362,8 +36945,22 @@
         <f>VLOOKUP(A113,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC113+VLOOKUP(A113,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P113" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q113" s="2">
+        <f>VLOOKUP(A113,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>7506</v>
+      </c>
+      <c r="R113" t="s">
+        <v>442</v>
+      </c>
+      <c r="S113" s="6">
+        <f>VLOOKUP(A113,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>7506</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>199</v>
       </c>
@@ -35416,8 +37013,22 @@
         <f>VLOOKUP(A114,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC114+VLOOKUP(A114,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P114" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q114" s="2">
+        <f>VLOOKUP(A114,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1536</v>
+      </c>
+      <c r="R114" t="s">
+        <v>442</v>
+      </c>
+      <c r="S114" s="6">
+        <f>VLOOKUP(A114,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>200</v>
       </c>
@@ -35470,8 +37081,22 @@
         <f>VLOOKUP(A115,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC115+VLOOKUP(A115,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P115" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q115" s="2">
+        <f>VLOOKUP(A115,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1554</v>
+      </c>
+      <c r="R115" t="s">
+        <v>442</v>
+      </c>
+      <c r="S115" s="6">
+        <f>VLOOKUP(A115,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>201</v>
       </c>
@@ -35524,8 +37149,22 @@
         <f>VLOOKUP(A116,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC116+VLOOKUP(A116,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P116" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q116" s="2">
+        <f>VLOOKUP(A116,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1518</v>
+      </c>
+      <c r="R116" t="s">
+        <v>442</v>
+      </c>
+      <c r="S116" s="6">
+        <f>VLOOKUP(A116,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>202</v>
       </c>
@@ -35578,8 +37217,22 @@
         <f>VLOOKUP(A117,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC117+VLOOKUP(A117,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P117" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q117" s="2">
+        <f>VLOOKUP(A117,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1608</v>
+      </c>
+      <c r="R117" t="s">
+        <v>442</v>
+      </c>
+      <c r="S117" s="6">
+        <f>VLOOKUP(A117,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>203</v>
       </c>
@@ -35632,8 +37285,22 @@
         <f>VLOOKUP(A118,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC118+VLOOKUP(A118,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>10000</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P118" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q118" s="2">
+        <f>VLOOKUP(A118,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1200</v>
+      </c>
+      <c r="R118" t="s">
+        <v>442</v>
+      </c>
+      <c r="S118" s="6">
+        <f>VLOOKUP(A118,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>205</v>
       </c>
@@ -35686,8 +37353,22 @@
         <f>VLOOKUP(A119,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC119+VLOOKUP(A119,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P119" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q119" s="2">
+        <f>VLOOKUP(A119,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1602</v>
+      </c>
+      <c r="R119" t="s">
+        <v>442</v>
+      </c>
+      <c r="S119" s="6">
+        <f>VLOOKUP(A119,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>206</v>
       </c>
@@ -35740,8 +37421,22 @@
         <f>VLOOKUP(A120,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC120+VLOOKUP(A120,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P120" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q120" s="2">
+        <f>VLOOKUP(A120,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1572</v>
+      </c>
+      <c r="R120" t="s">
+        <v>442</v>
+      </c>
+      <c r="S120" s="6">
+        <f>VLOOKUP(A120,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>207</v>
       </c>
@@ -35794,8 +37489,22 @@
         <f>VLOOKUP(A121,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC121+VLOOKUP(A121,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P121" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q121" s="2">
+        <f>VLOOKUP(A121,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1548</v>
+      </c>
+      <c r="R121" t="s">
+        <v>442</v>
+      </c>
+      <c r="S121" s="6">
+        <f>VLOOKUP(A121,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>208</v>
       </c>
@@ -35848,8 +37557,22 @@
         <f>VLOOKUP(A122,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC122+VLOOKUP(A122,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P122" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q122" s="2">
+        <f>VLOOKUP(A122,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3690</v>
+      </c>
+      <c r="R122" t="s">
+        <v>442</v>
+      </c>
+      <c r="S122" s="6">
+        <f>VLOOKUP(A122,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>209</v>
       </c>
@@ -35902,8 +37625,22 @@
         <f>VLOOKUP(A123,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC123+VLOOKUP(A123,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P123" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q123" s="2">
+        <f>VLOOKUP(A123,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3995.9999999999995</v>
+      </c>
+      <c r="R123" t="s">
+        <v>442</v>
+      </c>
+      <c r="S123" s="6">
+        <f>VLOOKUP(A123,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3995.9999999999995</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>210</v>
       </c>
@@ -35956,8 +37693,22 @@
         <f>VLOOKUP(A124,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC124+VLOOKUP(A124,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P124" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q124" s="2">
+        <f>VLOOKUP(A124,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>6054</v>
+      </c>
+      <c r="R124" t="s">
+        <v>442</v>
+      </c>
+      <c r="S124" s="6">
+        <f>VLOOKUP(A124,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>6054</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>213</v>
       </c>
@@ -36010,8 +37761,22 @@
         <f>VLOOKUP(A125,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC125+VLOOKUP(A125,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P125" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q125" s="2">
+        <f>VLOOKUP(A125,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>6102</v>
+      </c>
+      <c r="R125" t="s">
+        <v>442</v>
+      </c>
+      <c r="S125" s="6">
+        <f>VLOOKUP(A125,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>6102</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>214</v>
       </c>
@@ -36064,8 +37829,22 @@
         <f>VLOOKUP(A126,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC126+VLOOKUP(A126,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P126" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q126" s="2">
+        <f>VLOOKUP(A126,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3786</v>
+      </c>
+      <c r="R126" t="s">
+        <v>442</v>
+      </c>
+      <c r="S126" s="6">
+        <f>VLOOKUP(A126,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3786</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>215</v>
       </c>
@@ -36118,8 +37897,22 @@
         <f>VLOOKUP(A127,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC127+VLOOKUP(A127,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P127" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q127" s="2">
+        <f>VLOOKUP(A127,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3924.0000000000005</v>
+      </c>
+      <c r="R127" t="s">
+        <v>442</v>
+      </c>
+      <c r="S127" s="6">
+        <f>VLOOKUP(A127,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3924.0000000000005</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>216</v>
       </c>
@@ -36172,8 +37965,22 @@
         <f>VLOOKUP(A128,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC128+VLOOKUP(A128,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P128" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q128" s="2">
+        <f>VLOOKUP(A128,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>4020</v>
+      </c>
+      <c r="R128" t="s">
+        <v>442</v>
+      </c>
+      <c r="S128" s="6">
+        <f>VLOOKUP(A128,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>217</v>
       </c>
@@ -36226,8 +38033,22 @@
         <f>VLOOKUP(A129,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC129+VLOOKUP(A129,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P129" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q129" s="2">
+        <f>VLOOKUP(A129,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3888</v>
+      </c>
+      <c r="R129" t="s">
+        <v>442</v>
+      </c>
+      <c r="S129" s="6">
+        <f>VLOOKUP(A129,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3888</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>218</v>
       </c>
@@ -36280,8 +38101,22 @@
         <f>VLOOKUP(A130,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC130+VLOOKUP(A130,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P130" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q130" s="2">
+        <f>VLOOKUP(A130,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3828</v>
+      </c>
+      <c r="R130" t="s">
+        <v>442</v>
+      </c>
+      <c r="S130" s="6">
+        <f>VLOOKUP(A130,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3828</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>219</v>
       </c>
@@ -36334,8 +38169,22 @@
         <f>VLOOKUP(A131,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC131+VLOOKUP(A131,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P131" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q131" s="2">
+        <f>VLOOKUP(A131,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3845.9999999999995</v>
+      </c>
+      <c r="R131" t="s">
+        <v>442</v>
+      </c>
+      <c r="S131" s="6">
+        <f>VLOOKUP(A131,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3845.9999999999995</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>220</v>
       </c>
@@ -36388,8 +38237,22 @@
         <f>VLOOKUP(A132,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC132+VLOOKUP(A132,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P132" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q132" s="2">
+        <f>VLOOKUP(A132,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3995.9999999999995</v>
+      </c>
+      <c r="R132" t="s">
+        <v>442</v>
+      </c>
+      <c r="S132" s="6">
+        <f>VLOOKUP(A132,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3995.9999999999995</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>221</v>
       </c>
@@ -36442,8 +38305,22 @@
         <f>VLOOKUP(A133,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC133+VLOOKUP(A133,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P133" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q133" s="2">
+        <f>VLOOKUP(A133,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3744</v>
+      </c>
+      <c r="R133" t="s">
+        <v>442</v>
+      </c>
+      <c r="S133" s="6">
+        <f>VLOOKUP(A133,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>222</v>
       </c>
@@ -36496,8 +38373,22 @@
         <f>VLOOKUP(A134,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC134+VLOOKUP(A134,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P134" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q134" s="2">
+        <f>VLOOKUP(A134,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>4014.0000000000005</v>
+      </c>
+      <c r="R134" t="s">
+        <v>442</v>
+      </c>
+      <c r="S134" s="6">
+        <f>VLOOKUP(A134,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>4014.0000000000005</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>223</v>
       </c>
@@ -36550,8 +38441,22 @@
         <f>VLOOKUP(A135,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC135+VLOOKUP(A135,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P135" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q135" s="2">
+        <f>VLOOKUP(A135,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3912</v>
+      </c>
+      <c r="R135" t="s">
+        <v>442</v>
+      </c>
+      <c r="S135" s="6">
+        <f>VLOOKUP(A135,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3912</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>224</v>
       </c>
@@ -36604,8 +38509,22 @@
         <f>VLOOKUP(A136,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC136+VLOOKUP(A136,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P136" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q136" s="2">
+        <f>VLOOKUP(A136,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1668</v>
+      </c>
+      <c r="R136" t="s">
+        <v>442</v>
+      </c>
+      <c r="S136" s="6">
+        <f>VLOOKUP(A136,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>225</v>
       </c>
@@ -36658,8 +38577,22 @@
         <f>VLOOKUP(A137,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC137+VLOOKUP(A137,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P137" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q137" s="2">
+        <f>VLOOKUP(A137,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1638</v>
+      </c>
+      <c r="R137" t="s">
+        <v>442</v>
+      </c>
+      <c r="S137" s="6">
+        <f>VLOOKUP(A137,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>226</v>
       </c>
@@ -36712,8 +38645,22 @@
         <f>VLOOKUP(A138,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC138+VLOOKUP(A138,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P138" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q138" s="2">
+        <f>VLOOKUP(A138,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1620</v>
+      </c>
+      <c r="R138" t="s">
+        <v>442</v>
+      </c>
+      <c r="S138" s="6">
+        <f>VLOOKUP(A138,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>227</v>
       </c>
@@ -36766,8 +38713,22 @@
         <f>VLOOKUP(A139,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC139+VLOOKUP(A139,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P139" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q139" s="2">
+        <f>VLOOKUP(A139,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1698</v>
+      </c>
+      <c r="R139" t="s">
+        <v>442</v>
+      </c>
+      <c r="S139" s="6">
+        <f>VLOOKUP(A139,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>228</v>
       </c>
@@ -36820,8 +38781,22 @@
         <f>VLOOKUP(A140,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC140+VLOOKUP(A140,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P140" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q140" s="2">
+        <f>VLOOKUP(A140,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1632</v>
+      </c>
+      <c r="R140" t="s">
+        <v>442</v>
+      </c>
+      <c r="S140" s="6">
+        <f>VLOOKUP(A140,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>229</v>
       </c>
@@ -36874,8 +38849,22 @@
         <f>VLOOKUP(A141,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC141+VLOOKUP(A141,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P141" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q141" s="2">
+        <f>VLOOKUP(A141,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1620</v>
+      </c>
+      <c r="R141" t="s">
+        <v>442</v>
+      </c>
+      <c r="S141" s="6">
+        <f>VLOOKUP(A141,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>230</v>
       </c>
@@ -36928,8 +38917,22 @@
         <f>VLOOKUP(A142,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC142+VLOOKUP(A142,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P142" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q142" s="2">
+        <f>VLOOKUP(A142,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1692</v>
+      </c>
+      <c r="R142" t="s">
+        <v>442</v>
+      </c>
+      <c r="S142" s="6">
+        <f>VLOOKUP(A142,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>231</v>
       </c>
@@ -36982,8 +38985,22 @@
         <f>VLOOKUP(A143,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC143+VLOOKUP(A143,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P143" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q143" s="2">
+        <f>VLOOKUP(A143,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>558</v>
+      </c>
+      <c r="R143" t="s">
+        <v>442</v>
+      </c>
+      <c r="S143" s="6">
+        <f>VLOOKUP(A143,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>232</v>
       </c>
@@ -37036,8 +39053,22 @@
         <f>VLOOKUP(A144,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC144+VLOOKUP(A144,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P144" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q144" s="2">
+        <f>VLOOKUP(A144,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>582</v>
+      </c>
+      <c r="R144" t="s">
+        <v>442</v>
+      </c>
+      <c r="S144" s="6">
+        <f>VLOOKUP(A144,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>582</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>233</v>
       </c>
@@ -37090,8 +39121,22 @@
         <f>VLOOKUP(A145,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC145+VLOOKUP(A145,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P145" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q145" s="2">
+        <f>VLOOKUP(A145,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>564</v>
+      </c>
+      <c r="R145" t="s">
+        <v>442</v>
+      </c>
+      <c r="S145" s="6">
+        <f>VLOOKUP(A145,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>234</v>
       </c>
@@ -37144,8 +39189,22 @@
         <f>VLOOKUP(A146,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC146+VLOOKUP(A146,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P146" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q146" s="2">
+        <f>VLOOKUP(A146,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>546</v>
+      </c>
+      <c r="R146" t="s">
+        <v>442</v>
+      </c>
+      <c r="S146" s="6">
+        <f>VLOOKUP(A146,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>546</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>235</v>
       </c>
@@ -37198,8 +39257,22 @@
         <f>VLOOKUP(A147,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC147+VLOOKUP(A147,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P147" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q147" s="2">
+        <f>VLOOKUP(A147,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>546</v>
+      </c>
+      <c r="R147" t="s">
+        <v>442</v>
+      </c>
+      <c r="S147" s="6">
+        <f>VLOOKUP(A147,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>546</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>236</v>
       </c>
@@ -37252,8 +39325,22 @@
         <f>VLOOKUP(A148,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC148+VLOOKUP(A148,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P148" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q148" s="2">
+        <f>VLOOKUP(A148,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>582</v>
+      </c>
+      <c r="R148" t="s">
+        <v>442</v>
+      </c>
+      <c r="S148" s="6">
+        <f>VLOOKUP(A148,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>582</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>237</v>
       </c>
@@ -37306,8 +39393,22 @@
         <f>VLOOKUP(A149,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC149+VLOOKUP(A149,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P149" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q149" s="2">
+        <f>VLOOKUP(A149,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>564</v>
+      </c>
+      <c r="R149" t="s">
+        <v>442</v>
+      </c>
+      <c r="S149" s="6">
+        <f>VLOOKUP(A149,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>238</v>
       </c>
@@ -37360,8 +39461,22 @@
         <f>VLOOKUP(A150,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC150+VLOOKUP(A150,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P150" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q150" s="2">
+        <f>VLOOKUP(A150,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>708</v>
+      </c>
+      <c r="R150" t="s">
+        <v>442</v>
+      </c>
+      <c r="S150" s="6">
+        <f>VLOOKUP(A150,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>708</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>239</v>
       </c>
@@ -37414,8 +39529,22 @@
         <f>VLOOKUP(A151,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC151+VLOOKUP(A151,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P151" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q151" s="2">
+        <f>VLOOKUP(A151,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>672</v>
+      </c>
+      <c r="R151" t="s">
+        <v>442</v>
+      </c>
+      <c r="S151" s="6">
+        <f>VLOOKUP(A151,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>672</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>240</v>
       </c>
@@ -37468,8 +39597,22 @@
         <f>VLOOKUP(A152,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC152+VLOOKUP(A152,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P152" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q152" s="2">
+        <f>VLOOKUP(A152,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>618</v>
+      </c>
+      <c r="R152" t="s">
+        <v>442</v>
+      </c>
+      <c r="S152" s="6">
+        <f>VLOOKUP(A152,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>618</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>241</v>
       </c>
@@ -37522,8 +39665,22 @@
         <f>VLOOKUP(A153,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC153+VLOOKUP(A153,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P153" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q153" s="2">
+        <f>VLOOKUP(A153,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>270</v>
+      </c>
+      <c r="R153" t="s">
+        <v>442</v>
+      </c>
+      <c r="S153" s="6">
+        <f>VLOOKUP(A153,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>242</v>
       </c>
@@ -37576,8 +39733,22 @@
         <f>VLOOKUP(A154,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC154+VLOOKUP(A154,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P154" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q154" s="2">
+        <f>VLOOKUP(A154,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>792</v>
+      </c>
+      <c r="R154" t="s">
+        <v>442</v>
+      </c>
+      <c r="S154" s="6">
+        <f>VLOOKUP(A154,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>792</v>
+      </c>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>243</v>
       </c>
@@ -37630,8 +39801,22 @@
         <f>VLOOKUP(A155,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC155+VLOOKUP(A155,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P155" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q155" s="2">
+        <f>VLOOKUP(A155,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>8898</v>
+      </c>
+      <c r="R155" t="s">
+        <v>442</v>
+      </c>
+      <c r="S155" s="6">
+        <f>VLOOKUP(A155,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>8898</v>
+      </c>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>246</v>
       </c>
@@ -37684,8 +39869,22 @@
         <f>VLOOKUP(A156,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC156+VLOOKUP(A156,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P156" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q156" s="2">
+        <f>VLOOKUP(A156,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>47946</v>
+      </c>
+      <c r="R156" t="s">
+        <v>442</v>
+      </c>
+      <c r="S156" s="6">
+        <f>VLOOKUP(A156,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>47946</v>
+      </c>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>247</v>
       </c>
@@ -37738,8 +39937,22 @@
         <f>VLOOKUP(A157,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC157+VLOOKUP(A157,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P157" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q157" s="2">
+        <f>VLOOKUP(A157,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>50820</v>
+      </c>
+      <c r="R157" t="s">
+        <v>442</v>
+      </c>
+      <c r="S157" s="6">
+        <f>VLOOKUP(A157,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>50820</v>
+      </c>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>248</v>
       </c>
@@ -37792,8 +40005,22 @@
         <f>VLOOKUP(A158,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC158+VLOOKUP(A158,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P158" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q158" s="2">
+        <f>VLOOKUP(A158,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>42810</v>
+      </c>
+      <c r="R158" t="s">
+        <v>442</v>
+      </c>
+      <c r="S158" s="6">
+        <f>VLOOKUP(A158,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>42810</v>
+      </c>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>249</v>
       </c>
@@ -37845,6 +40072,20 @@
       <c r="O159" s="5">
         <f>VLOOKUP(A159,gen!$A$2:$BD$159,MATCH(gen!$U$1,gen!$1:$1,0),FALSE)*gen!AC159+VLOOKUP(A159,gen!$A$2:$BD$159,MATCH(gen!$X$1,gen!$1:$1,0),FALSE)</f>
         <v>0</v>
+      </c>
+      <c r="P159" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q159" s="2">
+        <f>VLOOKUP(A159,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
+      </c>
+      <c r="R159" t="s">
+        <v>442</v>
+      </c>
+      <c r="S159" s="6">
+        <f>VLOOKUP(A159,gen!$A$2:$BD$159,MATCH(gen!$Q$1,gen!$1:$1,0),FALSE)*60</f>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>
@@ -37857,7 +40098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3:F160"/>
     </sheetView>
   </sheetViews>
@@ -46862,8 +49103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H807"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E318" sqref="E318:E475"/>
+    <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
+      <selection activeCell="H630" sqref="H630"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56338,7 +58579,7 @@
         <v>0</v>
       </c>
       <c r="G451" t="str">
-        <f t="shared" ref="G451:G637" si="7">CONCATENATE("Region-",LEFT(B451,1))</f>
+        <f t="shared" ref="G451:G636" si="7">CONCATENATE("Region-",LEFT(B451,1))</f>
         <v>Region-3</v>
       </c>
     </row>
@@ -60244,7 +62485,7 @@
         <v>0</v>
       </c>
       <c r="G637" t="str">
-        <f t="shared" si="7"/>
+        <f>CONCATENATE("Region-",LEFT(B637,1))</f>
         <v>Region-3</v>
       </c>
     </row>
@@ -61408,8 +63649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H802"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D633" sqref="D633"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -70170,7 +72411,7 @@
         <v>0</v>
       </c>
       <c r="G417" t="str">
-        <f t="shared" ref="G417:G636" si="9">CONCATENATE("bus-",LEFT(B417,3))</f>
+        <f t="shared" ref="G417:G633" si="9">CONCATENATE("bus-",LEFT(B417,3))</f>
         <v>bus-313</v>
       </c>
     </row>
@@ -74664,7 +76905,7 @@
         <v>0</v>
       </c>
       <c r="G631" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("bus-",LEFT(B631,3))</f>
         <v>bus-303</v>
       </c>
     </row>
@@ -74727,7 +76968,7 @@
         <v>50</v>
       </c>
       <c r="G634" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G634:G637" si="10">CONCATENATE("bus-",LEFT(B634,3))</f>
         <v>bus-313</v>
       </c>
     </row>
@@ -74748,7 +76989,7 @@
         <v>0</v>
       </c>
       <c r="G635" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>bus-313</v>
       </c>
     </row>
@@ -74769,7 +77010,7 @@
         <v>0</v>
       </c>
       <c r="G636" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>bus-313</v>
       </c>
     </row>
@@ -74790,7 +77031,7 @@
         <v>0</v>
       </c>
       <c r="G637" t="str">
-        <f t="shared" ref="G637" si="10">CONCATENATE("bus-",LEFT(B637,3))</f>
+        <f t="shared" si="10"/>
         <v>bus-313</v>
       </c>
     </row>
@@ -75709,7 +77950,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="721" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="721" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A721" t="s">
         <v>434</v>
       </c>
@@ -75720,7 +77961,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="722" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="722" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A722" t="s">
         <v>434</v>
       </c>
@@ -75731,7 +77972,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="723" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="723" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A723" t="s">
         <v>434</v>
       </c>
@@ -75742,7 +77983,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="724" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="724" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A724" t="s">
         <v>434</v>
       </c>
@@ -75753,7 +77994,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="725" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="725" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A725" t="s">
         <v>434</v>
       </c>
@@ -75764,7 +78005,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="726" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="726" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A726" t="s">
         <v>434</v>
       </c>
@@ -75775,7 +78016,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="728" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="728" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A728" s="4" t="s">
         <v>433</v>
       </c>
@@ -75785,8 +78026,10 @@
       <c r="C728" s="4" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="729" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D728" s="4"/>
+      <c r="E728" s="4"/>
+    </row>
+    <row r="729" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A729" s="4" t="s">
         <v>433</v>
       </c>
@@ -75796,8 +78039,10 @@
       <c r="C729" s="4" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="730" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D729" s="4"/>
+      <c r="E729" s="4"/>
+    </row>
+    <row r="730" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A730" s="4" t="s">
         <v>433</v>
       </c>
@@ -75807,8 +78052,10 @@
       <c r="C730" s="4" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="731" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D730" s="4"/>
+      <c r="E730" s="4"/>
+    </row>
+    <row r="731" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A731" s="4" t="s">
         <v>434</v>
       </c>
@@ -75819,7 +78066,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="732" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="732" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A732" s="4" t="s">
         <v>434</v>
       </c>
@@ -75830,7 +78077,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="733" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="733" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A733" s="4" t="s">
         <v>434</v>
       </c>
@@ -75841,7 +78088,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="734" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="734" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A734" s="4" t="s">
         <v>434</v>
       </c>

</xml_diff>

<commit_message>
update to keep up with the SpineModel version
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/gen.xlsx
+++ b/spine_rts-gmlc/datasets/gen.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="gen" sheetId="1" r:id="rId1"/>
     <sheet name="Spine" sheetId="2" r:id="rId2"/>
     <sheet name="obj_unit" sheetId="12" r:id="rId3"/>
-    <sheet name="rel_unit__direction_node" sheetId="17" r:id="rId4"/>
-    <sheet name="rel_u__d_n-bus_detailed" sheetId="18" r:id="rId5"/>
-    <sheet name="rel_unit__node__node" sheetId="16" r:id="rId6"/>
-    <sheet name="rel_u__n__n-bus_detailed" sheetId="19" r:id="rId7"/>
+    <sheet name="rel_for_units_on_resolution" sheetId="20" r:id="rId4"/>
+    <sheet name="rel_unit__direction_node" sheetId="17" r:id="rId5"/>
+    <sheet name="rel_u__d_n-bus_detailed" sheetId="18" r:id="rId6"/>
+    <sheet name="rel_unit__node__node" sheetId="16" r:id="rId7"/>
+    <sheet name="rel_u__n__n-bus_detailed" sheetId="19" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">gen!$A$1:$BE$159</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10013" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10823" uniqueCount="451">
   <si>
     <t>GEN UID</t>
   </si>
@@ -1356,6 +1357,33 @@
   <si>
     <t>parameter_values</t>
   </si>
+  <si>
+    <t>unit_group__unit</t>
+  </si>
+  <si>
+    <t>all_units</t>
+  </si>
+  <si>
+    <t>units_on_resolution</t>
+  </si>
+  <si>
+    <t>node__temporal_block</t>
+  </si>
+  <si>
+    <t>temporal_block</t>
+  </si>
+  <si>
+    <t>object_class</t>
+  </si>
+  <si>
+    <t>object_name</t>
+  </si>
+  <si>
+    <t>blk_t1</t>
+  </si>
+  <si>
+    <t>blk_t2</t>
+  </si>
 </sst>
 </file>
 
@@ -40095,8 +40123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N171"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -46558,6 +46586,2782 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E162"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" t="s">
+        <v>444</v>
+      </c>
+      <c r="D3" t="s">
+        <v>446</v>
+      </c>
+      <c r="E3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" t="s">
+        <v>444</v>
+      </c>
+      <c r="D4" t="s">
+        <v>446</v>
+      </c>
+      <c r="E4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C5" t="s">
+        <v>443</v>
+      </c>
+      <c r="D5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>442</v>
+      </c>
+      <c r="B6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" t="s">
+        <v>443</v>
+      </c>
+      <c r="D6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>442</v>
+      </c>
+      <c r="B7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" t="s">
+        <v>443</v>
+      </c>
+      <c r="D7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>442</v>
+      </c>
+      <c r="B8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" t="s">
+        <v>443</v>
+      </c>
+      <c r="D8" t="s">
+        <v>262</v>
+      </c>
+      <c r="E8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>442</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9" t="s">
+        <v>443</v>
+      </c>
+      <c r="D9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>442</v>
+      </c>
+      <c r="B10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C10" t="s">
+        <v>443</v>
+      </c>
+      <c r="D10" t="s">
+        <v>262</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>442</v>
+      </c>
+      <c r="B11" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11" t="s">
+        <v>443</v>
+      </c>
+      <c r="D11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>442</v>
+      </c>
+      <c r="B12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C12" t="s">
+        <v>443</v>
+      </c>
+      <c r="D12" t="s">
+        <v>262</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>442</v>
+      </c>
+      <c r="B13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" t="s">
+        <v>443</v>
+      </c>
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>442</v>
+      </c>
+      <c r="B14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C14" t="s">
+        <v>443</v>
+      </c>
+      <c r="D14" t="s">
+        <v>262</v>
+      </c>
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>442</v>
+      </c>
+      <c r="B15" t="s">
+        <v>262</v>
+      </c>
+      <c r="C15" t="s">
+        <v>443</v>
+      </c>
+      <c r="D15" t="s">
+        <v>262</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>442</v>
+      </c>
+      <c r="B16" t="s">
+        <v>262</v>
+      </c>
+      <c r="C16" t="s">
+        <v>443</v>
+      </c>
+      <c r="D16" t="s">
+        <v>262</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>442</v>
+      </c>
+      <c r="B17" t="s">
+        <v>262</v>
+      </c>
+      <c r="C17" t="s">
+        <v>443</v>
+      </c>
+      <c r="D17" t="s">
+        <v>262</v>
+      </c>
+      <c r="E17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>442</v>
+      </c>
+      <c r="B18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" t="s">
+        <v>443</v>
+      </c>
+      <c r="D18" t="s">
+        <v>262</v>
+      </c>
+      <c r="E18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>442</v>
+      </c>
+      <c r="B19" t="s">
+        <v>262</v>
+      </c>
+      <c r="C19" t="s">
+        <v>443</v>
+      </c>
+      <c r="D19" t="s">
+        <v>262</v>
+      </c>
+      <c r="E19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>442</v>
+      </c>
+      <c r="B20" t="s">
+        <v>262</v>
+      </c>
+      <c r="C20" t="s">
+        <v>443</v>
+      </c>
+      <c r="D20" t="s">
+        <v>262</v>
+      </c>
+      <c r="E20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>442</v>
+      </c>
+      <c r="B21" t="s">
+        <v>262</v>
+      </c>
+      <c r="C21" t="s">
+        <v>443</v>
+      </c>
+      <c r="D21" t="s">
+        <v>262</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>442</v>
+      </c>
+      <c r="B22" t="s">
+        <v>262</v>
+      </c>
+      <c r="C22" t="s">
+        <v>443</v>
+      </c>
+      <c r="D22" t="s">
+        <v>262</v>
+      </c>
+      <c r="E22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>442</v>
+      </c>
+      <c r="B23" t="s">
+        <v>262</v>
+      </c>
+      <c r="C23" t="s">
+        <v>443</v>
+      </c>
+      <c r="D23" t="s">
+        <v>262</v>
+      </c>
+      <c r="E23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>442</v>
+      </c>
+      <c r="B24" t="s">
+        <v>262</v>
+      </c>
+      <c r="C24" t="s">
+        <v>443</v>
+      </c>
+      <c r="D24" t="s">
+        <v>262</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>442</v>
+      </c>
+      <c r="B25" t="s">
+        <v>262</v>
+      </c>
+      <c r="C25" t="s">
+        <v>443</v>
+      </c>
+      <c r="D25" t="s">
+        <v>262</v>
+      </c>
+      <c r="E25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>442</v>
+      </c>
+      <c r="B26" t="s">
+        <v>262</v>
+      </c>
+      <c r="C26" t="s">
+        <v>443</v>
+      </c>
+      <c r="D26" t="s">
+        <v>262</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>442</v>
+      </c>
+      <c r="B27" t="s">
+        <v>262</v>
+      </c>
+      <c r="C27" t="s">
+        <v>443</v>
+      </c>
+      <c r="D27" t="s">
+        <v>262</v>
+      </c>
+      <c r="E27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>442</v>
+      </c>
+      <c r="B28" t="s">
+        <v>262</v>
+      </c>
+      <c r="C28" t="s">
+        <v>443</v>
+      </c>
+      <c r="D28" t="s">
+        <v>262</v>
+      </c>
+      <c r="E28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>442</v>
+      </c>
+      <c r="B29" t="s">
+        <v>262</v>
+      </c>
+      <c r="C29" t="s">
+        <v>443</v>
+      </c>
+      <c r="D29" t="s">
+        <v>262</v>
+      </c>
+      <c r="E29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>442</v>
+      </c>
+      <c r="B30" t="s">
+        <v>262</v>
+      </c>
+      <c r="C30" t="s">
+        <v>443</v>
+      </c>
+      <c r="D30" t="s">
+        <v>262</v>
+      </c>
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>442</v>
+      </c>
+      <c r="B31" t="s">
+        <v>262</v>
+      </c>
+      <c r="C31" t="s">
+        <v>443</v>
+      </c>
+      <c r="D31" t="s">
+        <v>262</v>
+      </c>
+      <c r="E31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>442</v>
+      </c>
+      <c r="B32" t="s">
+        <v>262</v>
+      </c>
+      <c r="C32" t="s">
+        <v>443</v>
+      </c>
+      <c r="D32" t="s">
+        <v>262</v>
+      </c>
+      <c r="E32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>442</v>
+      </c>
+      <c r="B33" t="s">
+        <v>262</v>
+      </c>
+      <c r="C33" t="s">
+        <v>443</v>
+      </c>
+      <c r="D33" t="s">
+        <v>262</v>
+      </c>
+      <c r="E33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>442</v>
+      </c>
+      <c r="B34" t="s">
+        <v>262</v>
+      </c>
+      <c r="C34" t="s">
+        <v>443</v>
+      </c>
+      <c r="D34" t="s">
+        <v>262</v>
+      </c>
+      <c r="E34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>442</v>
+      </c>
+      <c r="B35" t="s">
+        <v>262</v>
+      </c>
+      <c r="C35" t="s">
+        <v>443</v>
+      </c>
+      <c r="D35" t="s">
+        <v>262</v>
+      </c>
+      <c r="E35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>442</v>
+      </c>
+      <c r="B36" t="s">
+        <v>262</v>
+      </c>
+      <c r="C36" t="s">
+        <v>443</v>
+      </c>
+      <c r="D36" t="s">
+        <v>262</v>
+      </c>
+      <c r="E36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>442</v>
+      </c>
+      <c r="B37" t="s">
+        <v>262</v>
+      </c>
+      <c r="C37" t="s">
+        <v>443</v>
+      </c>
+      <c r="D37" t="s">
+        <v>262</v>
+      </c>
+      <c r="E37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>442</v>
+      </c>
+      <c r="B38" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" t="s">
+        <v>443</v>
+      </c>
+      <c r="D38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>442</v>
+      </c>
+      <c r="B39" t="s">
+        <v>262</v>
+      </c>
+      <c r="C39" t="s">
+        <v>443</v>
+      </c>
+      <c r="D39" t="s">
+        <v>262</v>
+      </c>
+      <c r="E39" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>442</v>
+      </c>
+      <c r="B40" t="s">
+        <v>262</v>
+      </c>
+      <c r="C40" t="s">
+        <v>443</v>
+      </c>
+      <c r="D40" t="s">
+        <v>262</v>
+      </c>
+      <c r="E40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>442</v>
+      </c>
+      <c r="B41" t="s">
+        <v>262</v>
+      </c>
+      <c r="C41" t="s">
+        <v>443</v>
+      </c>
+      <c r="D41" t="s">
+        <v>262</v>
+      </c>
+      <c r="E41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>442</v>
+      </c>
+      <c r="B42" t="s">
+        <v>262</v>
+      </c>
+      <c r="C42" t="s">
+        <v>443</v>
+      </c>
+      <c r="D42" t="s">
+        <v>262</v>
+      </c>
+      <c r="E42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>442</v>
+      </c>
+      <c r="B43" t="s">
+        <v>262</v>
+      </c>
+      <c r="C43" t="s">
+        <v>443</v>
+      </c>
+      <c r="D43" t="s">
+        <v>262</v>
+      </c>
+      <c r="E43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>442</v>
+      </c>
+      <c r="B44" t="s">
+        <v>262</v>
+      </c>
+      <c r="C44" t="s">
+        <v>443</v>
+      </c>
+      <c r="D44" t="s">
+        <v>262</v>
+      </c>
+      <c r="E44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>442</v>
+      </c>
+      <c r="B45" t="s">
+        <v>262</v>
+      </c>
+      <c r="C45" t="s">
+        <v>443</v>
+      </c>
+      <c r="D45" t="s">
+        <v>262</v>
+      </c>
+      <c r="E45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>442</v>
+      </c>
+      <c r="B46" t="s">
+        <v>262</v>
+      </c>
+      <c r="C46" t="s">
+        <v>443</v>
+      </c>
+      <c r="D46" t="s">
+        <v>262</v>
+      </c>
+      <c r="E46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>442</v>
+      </c>
+      <c r="B47" t="s">
+        <v>262</v>
+      </c>
+      <c r="C47" t="s">
+        <v>443</v>
+      </c>
+      <c r="D47" t="s">
+        <v>262</v>
+      </c>
+      <c r="E47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>442</v>
+      </c>
+      <c r="B48" t="s">
+        <v>262</v>
+      </c>
+      <c r="C48" t="s">
+        <v>443</v>
+      </c>
+      <c r="D48" t="s">
+        <v>262</v>
+      </c>
+      <c r="E48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>442</v>
+      </c>
+      <c r="B49" t="s">
+        <v>262</v>
+      </c>
+      <c r="C49" t="s">
+        <v>443</v>
+      </c>
+      <c r="D49" t="s">
+        <v>262</v>
+      </c>
+      <c r="E49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>442</v>
+      </c>
+      <c r="B50" t="s">
+        <v>262</v>
+      </c>
+      <c r="C50" t="s">
+        <v>443</v>
+      </c>
+      <c r="D50" t="s">
+        <v>262</v>
+      </c>
+      <c r="E50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>442</v>
+      </c>
+      <c r="B51" t="s">
+        <v>262</v>
+      </c>
+      <c r="C51" t="s">
+        <v>443</v>
+      </c>
+      <c r="D51" t="s">
+        <v>262</v>
+      </c>
+      <c r="E51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>442</v>
+      </c>
+      <c r="B52" t="s">
+        <v>262</v>
+      </c>
+      <c r="C52" t="s">
+        <v>443</v>
+      </c>
+      <c r="D52" t="s">
+        <v>262</v>
+      </c>
+      <c r="E52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>442</v>
+      </c>
+      <c r="B53" t="s">
+        <v>262</v>
+      </c>
+      <c r="C53" t="s">
+        <v>443</v>
+      </c>
+      <c r="D53" t="s">
+        <v>262</v>
+      </c>
+      <c r="E53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>442</v>
+      </c>
+      <c r="B54" t="s">
+        <v>262</v>
+      </c>
+      <c r="C54" t="s">
+        <v>443</v>
+      </c>
+      <c r="D54" t="s">
+        <v>262</v>
+      </c>
+      <c r="E54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>442</v>
+      </c>
+      <c r="B55" t="s">
+        <v>262</v>
+      </c>
+      <c r="C55" t="s">
+        <v>443</v>
+      </c>
+      <c r="D55" t="s">
+        <v>262</v>
+      </c>
+      <c r="E55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>442</v>
+      </c>
+      <c r="B56" t="s">
+        <v>262</v>
+      </c>
+      <c r="C56" t="s">
+        <v>443</v>
+      </c>
+      <c r="D56" t="s">
+        <v>262</v>
+      </c>
+      <c r="E56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>442</v>
+      </c>
+      <c r="B57" t="s">
+        <v>262</v>
+      </c>
+      <c r="C57" t="s">
+        <v>443</v>
+      </c>
+      <c r="D57" t="s">
+        <v>262</v>
+      </c>
+      <c r="E57" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>442</v>
+      </c>
+      <c r="B58" t="s">
+        <v>262</v>
+      </c>
+      <c r="C58" t="s">
+        <v>443</v>
+      </c>
+      <c r="D58" t="s">
+        <v>262</v>
+      </c>
+      <c r="E58" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>442</v>
+      </c>
+      <c r="B59" t="s">
+        <v>262</v>
+      </c>
+      <c r="C59" t="s">
+        <v>443</v>
+      </c>
+      <c r="D59" t="s">
+        <v>262</v>
+      </c>
+      <c r="E59" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>442</v>
+      </c>
+      <c r="B60" t="s">
+        <v>262</v>
+      </c>
+      <c r="C60" t="s">
+        <v>443</v>
+      </c>
+      <c r="D60" t="s">
+        <v>262</v>
+      </c>
+      <c r="E60" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>442</v>
+      </c>
+      <c r="B61" t="s">
+        <v>262</v>
+      </c>
+      <c r="C61" t="s">
+        <v>443</v>
+      </c>
+      <c r="D61" t="s">
+        <v>262</v>
+      </c>
+      <c r="E61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>442</v>
+      </c>
+      <c r="B62" t="s">
+        <v>262</v>
+      </c>
+      <c r="C62" t="s">
+        <v>443</v>
+      </c>
+      <c r="D62" t="s">
+        <v>262</v>
+      </c>
+      <c r="E62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>442</v>
+      </c>
+      <c r="B63" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" t="s">
+        <v>443</v>
+      </c>
+      <c r="D63" t="s">
+        <v>262</v>
+      </c>
+      <c r="E63" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>442</v>
+      </c>
+      <c r="B64" t="s">
+        <v>262</v>
+      </c>
+      <c r="C64" t="s">
+        <v>443</v>
+      </c>
+      <c r="D64" t="s">
+        <v>262</v>
+      </c>
+      <c r="E64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>442</v>
+      </c>
+      <c r="B65" t="s">
+        <v>262</v>
+      </c>
+      <c r="C65" t="s">
+        <v>443</v>
+      </c>
+      <c r="D65" t="s">
+        <v>262</v>
+      </c>
+      <c r="E65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>442</v>
+      </c>
+      <c r="B66" t="s">
+        <v>262</v>
+      </c>
+      <c r="C66" t="s">
+        <v>443</v>
+      </c>
+      <c r="D66" t="s">
+        <v>262</v>
+      </c>
+      <c r="E66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>442</v>
+      </c>
+      <c r="B67" t="s">
+        <v>262</v>
+      </c>
+      <c r="C67" t="s">
+        <v>443</v>
+      </c>
+      <c r="D67" t="s">
+        <v>262</v>
+      </c>
+      <c r="E67" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>442</v>
+      </c>
+      <c r="B68" t="s">
+        <v>262</v>
+      </c>
+      <c r="C68" t="s">
+        <v>443</v>
+      </c>
+      <c r="D68" t="s">
+        <v>262</v>
+      </c>
+      <c r="E68" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>442</v>
+      </c>
+      <c r="B69" t="s">
+        <v>262</v>
+      </c>
+      <c r="C69" t="s">
+        <v>443</v>
+      </c>
+      <c r="D69" t="s">
+        <v>262</v>
+      </c>
+      <c r="E69" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>442</v>
+      </c>
+      <c r="B70" t="s">
+        <v>262</v>
+      </c>
+      <c r="C70" t="s">
+        <v>443</v>
+      </c>
+      <c r="D70" t="s">
+        <v>262</v>
+      </c>
+      <c r="E70" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>442</v>
+      </c>
+      <c r="B71" t="s">
+        <v>262</v>
+      </c>
+      <c r="C71" t="s">
+        <v>443</v>
+      </c>
+      <c r="D71" t="s">
+        <v>262</v>
+      </c>
+      <c r="E71" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>442</v>
+      </c>
+      <c r="B72" t="s">
+        <v>262</v>
+      </c>
+      <c r="C72" t="s">
+        <v>443</v>
+      </c>
+      <c r="D72" t="s">
+        <v>262</v>
+      </c>
+      <c r="E72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>442</v>
+      </c>
+      <c r="B73" t="s">
+        <v>262</v>
+      </c>
+      <c r="C73" t="s">
+        <v>443</v>
+      </c>
+      <c r="D73" t="s">
+        <v>262</v>
+      </c>
+      <c r="E73" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>442</v>
+      </c>
+      <c r="B74" t="s">
+        <v>262</v>
+      </c>
+      <c r="C74" t="s">
+        <v>443</v>
+      </c>
+      <c r="D74" t="s">
+        <v>262</v>
+      </c>
+      <c r="E74" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>442</v>
+      </c>
+      <c r="B75" t="s">
+        <v>262</v>
+      </c>
+      <c r="C75" t="s">
+        <v>443</v>
+      </c>
+      <c r="D75" t="s">
+        <v>262</v>
+      </c>
+      <c r="E75" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>442</v>
+      </c>
+      <c r="B76" t="s">
+        <v>262</v>
+      </c>
+      <c r="C76" t="s">
+        <v>443</v>
+      </c>
+      <c r="D76" t="s">
+        <v>262</v>
+      </c>
+      <c r="E76" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>442</v>
+      </c>
+      <c r="B77" t="s">
+        <v>262</v>
+      </c>
+      <c r="C77" t="s">
+        <v>443</v>
+      </c>
+      <c r="D77" t="s">
+        <v>262</v>
+      </c>
+      <c r="E77" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>442</v>
+      </c>
+      <c r="B78" t="s">
+        <v>262</v>
+      </c>
+      <c r="C78" t="s">
+        <v>443</v>
+      </c>
+      <c r="D78" t="s">
+        <v>262</v>
+      </c>
+      <c r="E78" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>442</v>
+      </c>
+      <c r="B79" t="s">
+        <v>262</v>
+      </c>
+      <c r="C79" t="s">
+        <v>443</v>
+      </c>
+      <c r="D79" t="s">
+        <v>262</v>
+      </c>
+      <c r="E79" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>442</v>
+      </c>
+      <c r="B80" t="s">
+        <v>262</v>
+      </c>
+      <c r="C80" t="s">
+        <v>443</v>
+      </c>
+      <c r="D80" t="s">
+        <v>262</v>
+      </c>
+      <c r="E80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>442</v>
+      </c>
+      <c r="B81" t="s">
+        <v>262</v>
+      </c>
+      <c r="C81" t="s">
+        <v>443</v>
+      </c>
+      <c r="D81" t="s">
+        <v>262</v>
+      </c>
+      <c r="E81" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>442</v>
+      </c>
+      <c r="B82" t="s">
+        <v>262</v>
+      </c>
+      <c r="C82" t="s">
+        <v>443</v>
+      </c>
+      <c r="D82" t="s">
+        <v>262</v>
+      </c>
+      <c r="E82" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>442</v>
+      </c>
+      <c r="B83" t="s">
+        <v>262</v>
+      </c>
+      <c r="C83" t="s">
+        <v>443</v>
+      </c>
+      <c r="D83" t="s">
+        <v>262</v>
+      </c>
+      <c r="E83" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>442</v>
+      </c>
+      <c r="B84" t="s">
+        <v>262</v>
+      </c>
+      <c r="C84" t="s">
+        <v>443</v>
+      </c>
+      <c r="D84" t="s">
+        <v>262</v>
+      </c>
+      <c r="E84" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>442</v>
+      </c>
+      <c r="B85" t="s">
+        <v>262</v>
+      </c>
+      <c r="C85" t="s">
+        <v>443</v>
+      </c>
+      <c r="D85" t="s">
+        <v>262</v>
+      </c>
+      <c r="E85" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>442</v>
+      </c>
+      <c r="B86" t="s">
+        <v>262</v>
+      </c>
+      <c r="C86" t="s">
+        <v>443</v>
+      </c>
+      <c r="D86" t="s">
+        <v>262</v>
+      </c>
+      <c r="E86" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>442</v>
+      </c>
+      <c r="B87" t="s">
+        <v>262</v>
+      </c>
+      <c r="C87" t="s">
+        <v>443</v>
+      </c>
+      <c r="D87" t="s">
+        <v>262</v>
+      </c>
+      <c r="E87" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>442</v>
+      </c>
+      <c r="B88" t="s">
+        <v>262</v>
+      </c>
+      <c r="C88" t="s">
+        <v>443</v>
+      </c>
+      <c r="D88" t="s">
+        <v>262</v>
+      </c>
+      <c r="E88" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>442</v>
+      </c>
+      <c r="B89" t="s">
+        <v>262</v>
+      </c>
+      <c r="C89" t="s">
+        <v>443</v>
+      </c>
+      <c r="D89" t="s">
+        <v>262</v>
+      </c>
+      <c r="E89" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>442</v>
+      </c>
+      <c r="B90" t="s">
+        <v>262</v>
+      </c>
+      <c r="C90" t="s">
+        <v>443</v>
+      </c>
+      <c r="D90" t="s">
+        <v>262</v>
+      </c>
+      <c r="E90" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>442</v>
+      </c>
+      <c r="B91" t="s">
+        <v>262</v>
+      </c>
+      <c r="C91" t="s">
+        <v>443</v>
+      </c>
+      <c r="D91" t="s">
+        <v>262</v>
+      </c>
+      <c r="E91" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>442</v>
+      </c>
+      <c r="B92" t="s">
+        <v>262</v>
+      </c>
+      <c r="C92" t="s">
+        <v>443</v>
+      </c>
+      <c r="D92" t="s">
+        <v>262</v>
+      </c>
+      <c r="E92" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>442</v>
+      </c>
+      <c r="B93" t="s">
+        <v>262</v>
+      </c>
+      <c r="C93" t="s">
+        <v>443</v>
+      </c>
+      <c r="D93" t="s">
+        <v>262</v>
+      </c>
+      <c r="E93" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>442</v>
+      </c>
+      <c r="B94" t="s">
+        <v>262</v>
+      </c>
+      <c r="C94" t="s">
+        <v>443</v>
+      </c>
+      <c r="D94" t="s">
+        <v>262</v>
+      </c>
+      <c r="E94" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>442</v>
+      </c>
+      <c r="B95" t="s">
+        <v>262</v>
+      </c>
+      <c r="C95" t="s">
+        <v>443</v>
+      </c>
+      <c r="D95" t="s">
+        <v>262</v>
+      </c>
+      <c r="E95" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>442</v>
+      </c>
+      <c r="B96" t="s">
+        <v>262</v>
+      </c>
+      <c r="C96" t="s">
+        <v>443</v>
+      </c>
+      <c r="D96" t="s">
+        <v>262</v>
+      </c>
+      <c r="E96" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>442</v>
+      </c>
+      <c r="B97" t="s">
+        <v>262</v>
+      </c>
+      <c r="C97" t="s">
+        <v>443</v>
+      </c>
+      <c r="D97" t="s">
+        <v>262</v>
+      </c>
+      <c r="E97" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>442</v>
+      </c>
+      <c r="B98" t="s">
+        <v>262</v>
+      </c>
+      <c r="C98" t="s">
+        <v>443</v>
+      </c>
+      <c r="D98" t="s">
+        <v>262</v>
+      </c>
+      <c r="E98" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>442</v>
+      </c>
+      <c r="B99" t="s">
+        <v>262</v>
+      </c>
+      <c r="C99" t="s">
+        <v>443</v>
+      </c>
+      <c r="D99" t="s">
+        <v>262</v>
+      </c>
+      <c r="E99" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>442</v>
+      </c>
+      <c r="B100" t="s">
+        <v>262</v>
+      </c>
+      <c r="C100" t="s">
+        <v>443</v>
+      </c>
+      <c r="D100" t="s">
+        <v>262</v>
+      </c>
+      <c r="E100" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>442</v>
+      </c>
+      <c r="B101" t="s">
+        <v>262</v>
+      </c>
+      <c r="C101" t="s">
+        <v>443</v>
+      </c>
+      <c r="D101" t="s">
+        <v>262</v>
+      </c>
+      <c r="E101" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>442</v>
+      </c>
+      <c r="B102" t="s">
+        <v>262</v>
+      </c>
+      <c r="C102" t="s">
+        <v>443</v>
+      </c>
+      <c r="D102" t="s">
+        <v>262</v>
+      </c>
+      <c r="E102" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>442</v>
+      </c>
+      <c r="B103" t="s">
+        <v>262</v>
+      </c>
+      <c r="C103" t="s">
+        <v>443</v>
+      </c>
+      <c r="D103" t="s">
+        <v>262</v>
+      </c>
+      <c r="E103" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>442</v>
+      </c>
+      <c r="B104" t="s">
+        <v>262</v>
+      </c>
+      <c r="C104" t="s">
+        <v>443</v>
+      </c>
+      <c r="D104" t="s">
+        <v>262</v>
+      </c>
+      <c r="E104" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>442</v>
+      </c>
+      <c r="B105" t="s">
+        <v>262</v>
+      </c>
+      <c r="C105" t="s">
+        <v>443</v>
+      </c>
+      <c r="D105" t="s">
+        <v>262</v>
+      </c>
+      <c r="E105" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>442</v>
+      </c>
+      <c r="B106" t="s">
+        <v>262</v>
+      </c>
+      <c r="C106" t="s">
+        <v>443</v>
+      </c>
+      <c r="D106" t="s">
+        <v>262</v>
+      </c>
+      <c r="E106" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>442</v>
+      </c>
+      <c r="B107" t="s">
+        <v>262</v>
+      </c>
+      <c r="C107" t="s">
+        <v>443</v>
+      </c>
+      <c r="D107" t="s">
+        <v>262</v>
+      </c>
+      <c r="E107" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>442</v>
+      </c>
+      <c r="B108" t="s">
+        <v>262</v>
+      </c>
+      <c r="C108" t="s">
+        <v>443</v>
+      </c>
+      <c r="D108" t="s">
+        <v>262</v>
+      </c>
+      <c r="E108" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>442</v>
+      </c>
+      <c r="B109" t="s">
+        <v>262</v>
+      </c>
+      <c r="C109" t="s">
+        <v>443</v>
+      </c>
+      <c r="D109" t="s">
+        <v>262</v>
+      </c>
+      <c r="E109" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>442</v>
+      </c>
+      <c r="B110" t="s">
+        <v>262</v>
+      </c>
+      <c r="C110" t="s">
+        <v>443</v>
+      </c>
+      <c r="D110" t="s">
+        <v>262</v>
+      </c>
+      <c r="E110" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>442</v>
+      </c>
+      <c r="B111" t="s">
+        <v>262</v>
+      </c>
+      <c r="C111" t="s">
+        <v>443</v>
+      </c>
+      <c r="D111" t="s">
+        <v>262</v>
+      </c>
+      <c r="E111" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>442</v>
+      </c>
+      <c r="B112" t="s">
+        <v>262</v>
+      </c>
+      <c r="C112" t="s">
+        <v>443</v>
+      </c>
+      <c r="D112" t="s">
+        <v>262</v>
+      </c>
+      <c r="E112" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>442</v>
+      </c>
+      <c r="B113" t="s">
+        <v>262</v>
+      </c>
+      <c r="C113" t="s">
+        <v>443</v>
+      </c>
+      <c r="D113" t="s">
+        <v>262</v>
+      </c>
+      <c r="E113" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>442</v>
+      </c>
+      <c r="B114" t="s">
+        <v>262</v>
+      </c>
+      <c r="C114" t="s">
+        <v>443</v>
+      </c>
+      <c r="D114" t="s">
+        <v>262</v>
+      </c>
+      <c r="E114" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>442</v>
+      </c>
+      <c r="B115" t="s">
+        <v>262</v>
+      </c>
+      <c r="C115" t="s">
+        <v>443</v>
+      </c>
+      <c r="D115" t="s">
+        <v>262</v>
+      </c>
+      <c r="E115" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>442</v>
+      </c>
+      <c r="B116" t="s">
+        <v>262</v>
+      </c>
+      <c r="C116" t="s">
+        <v>443</v>
+      </c>
+      <c r="D116" t="s">
+        <v>262</v>
+      </c>
+      <c r="E116" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>442</v>
+      </c>
+      <c r="B117" t="s">
+        <v>262</v>
+      </c>
+      <c r="C117" t="s">
+        <v>443</v>
+      </c>
+      <c r="D117" t="s">
+        <v>262</v>
+      </c>
+      <c r="E117" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>442</v>
+      </c>
+      <c r="B118" t="s">
+        <v>262</v>
+      </c>
+      <c r="C118" t="s">
+        <v>443</v>
+      </c>
+      <c r="D118" t="s">
+        <v>262</v>
+      </c>
+      <c r="E118" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>442</v>
+      </c>
+      <c r="B119" t="s">
+        <v>262</v>
+      </c>
+      <c r="C119" t="s">
+        <v>443</v>
+      </c>
+      <c r="D119" t="s">
+        <v>262</v>
+      </c>
+      <c r="E119" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>442</v>
+      </c>
+      <c r="B120" t="s">
+        <v>262</v>
+      </c>
+      <c r="C120" t="s">
+        <v>443</v>
+      </c>
+      <c r="D120" t="s">
+        <v>262</v>
+      </c>
+      <c r="E120" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>442</v>
+      </c>
+      <c r="B121" t="s">
+        <v>262</v>
+      </c>
+      <c r="C121" t="s">
+        <v>443</v>
+      </c>
+      <c r="D121" t="s">
+        <v>262</v>
+      </c>
+      <c r="E121" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>442</v>
+      </c>
+      <c r="B122" t="s">
+        <v>262</v>
+      </c>
+      <c r="C122" t="s">
+        <v>443</v>
+      </c>
+      <c r="D122" t="s">
+        <v>262</v>
+      </c>
+      <c r="E122" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>442</v>
+      </c>
+      <c r="B123" t="s">
+        <v>262</v>
+      </c>
+      <c r="C123" t="s">
+        <v>443</v>
+      </c>
+      <c r="D123" t="s">
+        <v>262</v>
+      </c>
+      <c r="E123" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>442</v>
+      </c>
+      <c r="B124" t="s">
+        <v>262</v>
+      </c>
+      <c r="C124" t="s">
+        <v>443</v>
+      </c>
+      <c r="D124" t="s">
+        <v>262</v>
+      </c>
+      <c r="E124" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>442</v>
+      </c>
+      <c r="B125" t="s">
+        <v>262</v>
+      </c>
+      <c r="C125" t="s">
+        <v>443</v>
+      </c>
+      <c r="D125" t="s">
+        <v>262</v>
+      </c>
+      <c r="E125" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>442</v>
+      </c>
+      <c r="B126" t="s">
+        <v>262</v>
+      </c>
+      <c r="C126" t="s">
+        <v>443</v>
+      </c>
+      <c r="D126" t="s">
+        <v>262</v>
+      </c>
+      <c r="E126" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>442</v>
+      </c>
+      <c r="B127" t="s">
+        <v>262</v>
+      </c>
+      <c r="C127" t="s">
+        <v>443</v>
+      </c>
+      <c r="D127" t="s">
+        <v>262</v>
+      </c>
+      <c r="E127" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>442</v>
+      </c>
+      <c r="B128" t="s">
+        <v>262</v>
+      </c>
+      <c r="C128" t="s">
+        <v>443</v>
+      </c>
+      <c r="D128" t="s">
+        <v>262</v>
+      </c>
+      <c r="E128" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>442</v>
+      </c>
+      <c r="B129" t="s">
+        <v>262</v>
+      </c>
+      <c r="C129" t="s">
+        <v>443</v>
+      </c>
+      <c r="D129" t="s">
+        <v>262</v>
+      </c>
+      <c r="E129" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>442</v>
+      </c>
+      <c r="B130" t="s">
+        <v>262</v>
+      </c>
+      <c r="C130" t="s">
+        <v>443</v>
+      </c>
+      <c r="D130" t="s">
+        <v>262</v>
+      </c>
+      <c r="E130" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>442</v>
+      </c>
+      <c r="B131" t="s">
+        <v>262</v>
+      </c>
+      <c r="C131" t="s">
+        <v>443</v>
+      </c>
+      <c r="D131" t="s">
+        <v>262</v>
+      </c>
+      <c r="E131" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>442</v>
+      </c>
+      <c r="B132" t="s">
+        <v>262</v>
+      </c>
+      <c r="C132" t="s">
+        <v>443</v>
+      </c>
+      <c r="D132" t="s">
+        <v>262</v>
+      </c>
+      <c r="E132" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>442</v>
+      </c>
+      <c r="B133" t="s">
+        <v>262</v>
+      </c>
+      <c r="C133" t="s">
+        <v>443</v>
+      </c>
+      <c r="D133" t="s">
+        <v>262</v>
+      </c>
+      <c r="E133" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>442</v>
+      </c>
+      <c r="B134" t="s">
+        <v>262</v>
+      </c>
+      <c r="C134" t="s">
+        <v>443</v>
+      </c>
+      <c r="D134" t="s">
+        <v>262</v>
+      </c>
+      <c r="E134" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>442</v>
+      </c>
+      <c r="B135" t="s">
+        <v>262</v>
+      </c>
+      <c r="C135" t="s">
+        <v>443</v>
+      </c>
+      <c r="D135" t="s">
+        <v>262</v>
+      </c>
+      <c r="E135" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>442</v>
+      </c>
+      <c r="B136" t="s">
+        <v>262</v>
+      </c>
+      <c r="C136" t="s">
+        <v>443</v>
+      </c>
+      <c r="D136" t="s">
+        <v>262</v>
+      </c>
+      <c r="E136" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>442</v>
+      </c>
+      <c r="B137" t="s">
+        <v>262</v>
+      </c>
+      <c r="C137" t="s">
+        <v>443</v>
+      </c>
+      <c r="D137" t="s">
+        <v>262</v>
+      </c>
+      <c r="E137" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>442</v>
+      </c>
+      <c r="B138" t="s">
+        <v>262</v>
+      </c>
+      <c r="C138" t="s">
+        <v>443</v>
+      </c>
+      <c r="D138" t="s">
+        <v>262</v>
+      </c>
+      <c r="E138" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>442</v>
+      </c>
+      <c r="B139" t="s">
+        <v>262</v>
+      </c>
+      <c r="C139" t="s">
+        <v>443</v>
+      </c>
+      <c r="D139" t="s">
+        <v>262</v>
+      </c>
+      <c r="E139" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>442</v>
+      </c>
+      <c r="B140" t="s">
+        <v>262</v>
+      </c>
+      <c r="C140" t="s">
+        <v>443</v>
+      </c>
+      <c r="D140" t="s">
+        <v>262</v>
+      </c>
+      <c r="E140" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>442</v>
+      </c>
+      <c r="B141" t="s">
+        <v>262</v>
+      </c>
+      <c r="C141" t="s">
+        <v>443</v>
+      </c>
+      <c r="D141" t="s">
+        <v>262</v>
+      </c>
+      <c r="E141" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>442</v>
+      </c>
+      <c r="B142" t="s">
+        <v>262</v>
+      </c>
+      <c r="C142" t="s">
+        <v>443</v>
+      </c>
+      <c r="D142" t="s">
+        <v>262</v>
+      </c>
+      <c r="E142" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>442</v>
+      </c>
+      <c r="B143" t="s">
+        <v>262</v>
+      </c>
+      <c r="C143" t="s">
+        <v>443</v>
+      </c>
+      <c r="D143" t="s">
+        <v>262</v>
+      </c>
+      <c r="E143" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>442</v>
+      </c>
+      <c r="B144" t="s">
+        <v>262</v>
+      </c>
+      <c r="C144" t="s">
+        <v>443</v>
+      </c>
+      <c r="D144" t="s">
+        <v>262</v>
+      </c>
+      <c r="E144" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>442</v>
+      </c>
+      <c r="B145" t="s">
+        <v>262</v>
+      </c>
+      <c r="C145" t="s">
+        <v>443</v>
+      </c>
+      <c r="D145" t="s">
+        <v>262</v>
+      </c>
+      <c r="E145" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>442</v>
+      </c>
+      <c r="B146" t="s">
+        <v>262</v>
+      </c>
+      <c r="C146" t="s">
+        <v>443</v>
+      </c>
+      <c r="D146" t="s">
+        <v>262</v>
+      </c>
+      <c r="E146" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>442</v>
+      </c>
+      <c r="B147" t="s">
+        <v>262</v>
+      </c>
+      <c r="C147" t="s">
+        <v>443</v>
+      </c>
+      <c r="D147" t="s">
+        <v>262</v>
+      </c>
+      <c r="E147" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>442</v>
+      </c>
+      <c r="B148" t="s">
+        <v>262</v>
+      </c>
+      <c r="C148" t="s">
+        <v>443</v>
+      </c>
+      <c r="D148" t="s">
+        <v>262</v>
+      </c>
+      <c r="E148" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>442</v>
+      </c>
+      <c r="B149" t="s">
+        <v>262</v>
+      </c>
+      <c r="C149" t="s">
+        <v>443</v>
+      </c>
+      <c r="D149" t="s">
+        <v>262</v>
+      </c>
+      <c r="E149" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>442</v>
+      </c>
+      <c r="B150" t="s">
+        <v>262</v>
+      </c>
+      <c r="C150" t="s">
+        <v>443</v>
+      </c>
+      <c r="D150" t="s">
+        <v>262</v>
+      </c>
+      <c r="E150" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>442</v>
+      </c>
+      <c r="B151" t="s">
+        <v>262</v>
+      </c>
+      <c r="C151" t="s">
+        <v>443</v>
+      </c>
+      <c r="D151" t="s">
+        <v>262</v>
+      </c>
+      <c r="E151" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>442</v>
+      </c>
+      <c r="B152" t="s">
+        <v>262</v>
+      </c>
+      <c r="C152" t="s">
+        <v>443</v>
+      </c>
+      <c r="D152" t="s">
+        <v>262</v>
+      </c>
+      <c r="E152" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>442</v>
+      </c>
+      <c r="B153" t="s">
+        <v>262</v>
+      </c>
+      <c r="C153" t="s">
+        <v>443</v>
+      </c>
+      <c r="D153" t="s">
+        <v>262</v>
+      </c>
+      <c r="E153" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>442</v>
+      </c>
+      <c r="B154" t="s">
+        <v>262</v>
+      </c>
+      <c r="C154" t="s">
+        <v>443</v>
+      </c>
+      <c r="D154" t="s">
+        <v>262</v>
+      </c>
+      <c r="E154" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>442</v>
+      </c>
+      <c r="B155" t="s">
+        <v>262</v>
+      </c>
+      <c r="C155" t="s">
+        <v>443</v>
+      </c>
+      <c r="D155" t="s">
+        <v>262</v>
+      </c>
+      <c r="E155" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>442</v>
+      </c>
+      <c r="B156" t="s">
+        <v>262</v>
+      </c>
+      <c r="C156" t="s">
+        <v>443</v>
+      </c>
+      <c r="D156" t="s">
+        <v>262</v>
+      </c>
+      <c r="E156" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>442</v>
+      </c>
+      <c r="B157" t="s">
+        <v>262</v>
+      </c>
+      <c r="C157" t="s">
+        <v>443</v>
+      </c>
+      <c r="D157" t="s">
+        <v>262</v>
+      </c>
+      <c r="E157" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>442</v>
+      </c>
+      <c r="B158" t="s">
+        <v>262</v>
+      </c>
+      <c r="C158" t="s">
+        <v>443</v>
+      </c>
+      <c r="D158" t="s">
+        <v>262</v>
+      </c>
+      <c r="E158" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>442</v>
+      </c>
+      <c r="B159" t="s">
+        <v>262</v>
+      </c>
+      <c r="C159" t="s">
+        <v>443</v>
+      </c>
+      <c r="D159" t="s">
+        <v>262</v>
+      </c>
+      <c r="E159" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>442</v>
+      </c>
+      <c r="B160" t="s">
+        <v>262</v>
+      </c>
+      <c r="C160" t="s">
+        <v>443</v>
+      </c>
+      <c r="D160" t="s">
+        <v>262</v>
+      </c>
+      <c r="E160" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>442</v>
+      </c>
+      <c r="B161" t="s">
+        <v>262</v>
+      </c>
+      <c r="C161" t="s">
+        <v>443</v>
+      </c>
+      <c r="D161" t="s">
+        <v>262</v>
+      </c>
+      <c r="E161" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>442</v>
+      </c>
+      <c r="B162" t="s">
+        <v>262</v>
+      </c>
+      <c r="C162" t="s">
+        <v>443</v>
+      </c>
+      <c r="D162" t="s">
+        <v>262</v>
+      </c>
+      <c r="E162" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H807"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -61102,7 +63906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H802"/>
   <sheetViews>
@@ -75564,7 +78368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H82"/>
   <sheetViews>
@@ -77552,11 +80356,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>